<commit_message>
opdateret dataset og inkluderet nye ligninger i model
</commit_message>
<xml_diff>
--- a/AAMK.xlsx
+++ b/AAMK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaudk-my.sharepoint.com/personal/rs_id_aau_dk/Documents/AAU/06 Current Projects/00 SFC Quarterly - data - DK SE NO FI/SFCmodel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjkss\Desktop\9. semester\Empirisk-SFC-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{6B7ABB2B-C4C1-EF44-AA30-DDB4BD2979AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{438AAE37-7171-1C43-80A9-D3F173CFD55A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F94EC50-29CB-4DB5-8660-292DE0166CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="515">
   <si>
     <t>IBA_h</t>
   </si>
@@ -1569,6 +1569,15 @@
   <si>
     <t>cpi1</t>
   </si>
+  <si>
+    <t>Dagpenge</t>
+  </si>
+  <si>
+    <t>abm</t>
+  </si>
+  <si>
+    <t>ratio_dag</t>
+  </si>
 </sst>
 </file>
 
@@ -1633,13 +1642,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,7 +1671,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1954,16 +1967,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:QJ68"/>
+  <dimension ref="A1:QM68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="QG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="QJ7" sqref="QJ7"/>
+      <selection pane="topRight" activeCell="QN5" sqref="QN5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>496</v>
       </c>
@@ -3320,8 +3333,17 @@
       <c r="QJ1" t="s">
         <v>511</v>
       </c>
+      <c r="QK1" t="s">
+        <v>512</v>
+      </c>
+      <c r="QL1" t="s">
+        <v>513</v>
+      </c>
+      <c r="QM1" t="s">
+        <v>514</v>
+      </c>
     </row>
-    <row r="2" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -4678,8 +4700,17 @@
       <c r="QJ2">
         <v>89.95736181431883</v>
       </c>
+      <c r="QK2" s="6">
+        <v>5192.3019999999997</v>
+      </c>
+      <c r="QL2" s="7">
+        <v>16715</v>
+      </c>
+      <c r="QM2">
+        <v>6.8836489702304798E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>357</v>
       </c>
@@ -6036,8 +6067,17 @@
       <c r="QJ3">
         <v>90.135565815589473</v>
       </c>
+      <c r="QK3" s="6">
+        <v>5192.3019999999997</v>
+      </c>
+      <c r="QL3" s="7">
+        <v>17787</v>
+      </c>
+      <c r="QM3">
+        <v>6.8836489702304798E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -7394,8 +7434,17 @@
       <c r="QJ4">
         <v>90.385051331830496</v>
       </c>
+      <c r="QK4" s="6">
+        <v>5192.3019999999997</v>
+      </c>
+      <c r="QL4" s="7">
+        <v>17611</v>
+      </c>
+      <c r="QM4">
+        <v>6.8836489702304798E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -8752,8 +8801,17 @@
       <c r="QJ5">
         <v>90.705818469964285</v>
       </c>
+      <c r="QK5" s="6">
+        <v>4004.3744999999999</v>
+      </c>
+      <c r="QL5" s="7">
+        <v>17710</v>
+      </c>
+      <c r="QM5">
+        <v>5.229759432668573E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -10110,8 +10168,17 @@
       <c r="QJ6">
         <v>91.775042263743515</v>
       </c>
+      <c r="QK6" s="6">
+        <v>4004.3744999999999</v>
+      </c>
+      <c r="QL6" s="7">
+        <v>18553</v>
+      </c>
+      <c r="QM6">
+        <v>5.229759432668573E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -11468,8 +11535,17 @@
       <c r="QJ7">
         <v>91.846323885636252</v>
       </c>
+      <c r="QK7" s="6">
+        <v>4004.3744999999999</v>
+      </c>
+      <c r="QL7" s="7">
+        <v>17499</v>
+      </c>
+      <c r="QM7">
+        <v>5.229759432668573E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -12826,8 +12902,17 @@
       <c r="QJ8">
         <v>91.917605507529004</v>
       </c>
+      <c r="QK8" s="6">
+        <v>4004.3744999999999</v>
+      </c>
+      <c r="QL8" s="7">
+        <v>17923</v>
+      </c>
+      <c r="QM8">
+        <v>5.229759432668573E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>363</v>
       </c>
@@ -14184,8 +14269,17 @@
       <c r="QJ9">
         <v>92.41657654001105</v>
       </c>
+      <c r="QK9" s="6">
+        <v>2807.7310000000002</v>
+      </c>
+      <c r="QL9" s="7">
+        <v>18802</v>
+      </c>
+      <c r="QM9">
+        <v>3.6330512531863417E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -15542,8 +15636,17 @@
       <c r="QJ10">
         <v>93.236314817549257</v>
       </c>
+      <c r="QK10" s="6">
+        <v>2807.7310000000002</v>
+      </c>
+      <c r="QL10" s="7">
+        <v>18159</v>
+      </c>
+      <c r="QM10">
+        <v>3.6330512531863417E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>365</v>
       </c>
@@ -16900,8 +17003,17 @@
       <c r="QJ11">
         <v>92.879906921930285</v>
       </c>
+      <c r="QK11" s="6">
+        <v>2807.7310000000002</v>
+      </c>
+      <c r="QL11" s="7">
+        <v>20211</v>
+      </c>
+      <c r="QM11">
+        <v>3.6330512531863417E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -18258,8 +18370,17 @@
       <c r="QJ12">
         <v>93.913489851301989</v>
       </c>
+      <c r="QK12" s="6">
+        <v>2807.7310000000002</v>
+      </c>
+      <c r="QL12" s="7">
+        <v>19436</v>
+      </c>
+      <c r="QM12">
+        <v>3.6330512531863417E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>367</v>
       </c>
@@ -19616,8 +19737,17 @@
       <c r="QJ13">
         <v>95.232199268244628</v>
       </c>
+      <c r="QK13" s="6">
+        <v>1932.4655</v>
+      </c>
+      <c r="QL13" s="7">
+        <v>17969</v>
+      </c>
+      <c r="QM13">
+        <v>2.4640780103410243E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -20974,8 +21104,17 @@
       <c r="QJ14">
         <v>96.515267820779712</v>
       </c>
+      <c r="QK14" s="6">
+        <v>1932.4655</v>
+      </c>
+      <c r="QL14" s="7">
+        <v>20815</v>
+      </c>
+      <c r="QM14">
+        <v>2.4640780103410243E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>369</v>
       </c>
@@ -22332,8 +22471,17 @@
       <c r="QJ15">
         <v>96.764753337020736</v>
       </c>
+      <c r="QK15" s="6">
+        <v>1932.4655</v>
+      </c>
+      <c r="QL15" s="7">
+        <v>20385</v>
+      </c>
+      <c r="QM15">
+        <v>2.4640780103410243E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>370</v>
       </c>
@@ -23690,8 +23838,17 @@
       <c r="QJ16">
         <v>96.657830957642801</v>
       </c>
+      <c r="QK16" s="6">
+        <v>1932.4655</v>
+      </c>
+      <c r="QL16" s="7">
+        <v>21117</v>
+      </c>
+      <c r="QM16">
+        <v>2.4640780103410243E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>371</v>
       </c>
@@ -25048,8 +25205,17 @@
       <c r="QJ17">
         <v>96.907316473883853</v>
       </c>
+      <c r="QK17" s="6">
+        <v>3860.5152499999999</v>
+      </c>
+      <c r="QL17" s="7">
+        <v>18969</v>
+      </c>
+      <c r="QM17">
+        <v>4.5142325513410804E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -26406,8 +26572,17 @@
       <c r="QJ18">
         <v>97.691413993936848</v>
       </c>
+      <c r="QK18" s="6">
+        <v>3860.5152499999999</v>
+      </c>
+      <c r="QL18" s="7">
+        <v>20287</v>
+      </c>
+      <c r="QM18">
+        <v>4.5142325513410804E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>373</v>
       </c>
@@ -27764,8 +27939,17 @@
       <c r="QJ19">
         <v>97.727054751422045</v>
       </c>
+      <c r="QK19" s="6">
+        <v>3860.5152499999999</v>
+      </c>
+      <c r="QL19" s="7">
+        <v>20185</v>
+      </c>
+      <c r="QM19">
+        <v>4.5142325513410804E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>374</v>
       </c>
@@ -29122,8 +29306,17 @@
       <c r="QJ20">
         <v>97.869617888285134</v>
       </c>
+      <c r="QK20" s="6">
+        <v>3860.5152499999999</v>
+      </c>
+      <c r="QL20" s="7">
+        <v>20186</v>
+      </c>
+      <c r="QM20">
+        <v>4.5142325513410804E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>375</v>
       </c>
@@ -30480,8 +30673,17 @@
       <c r="QJ21">
         <v>98.938841682064378</v>
       </c>
+      <c r="QK21" s="6">
+        <v>5154.2924999999996</v>
+      </c>
+      <c r="QL21" s="7">
+        <v>20012</v>
+      </c>
+      <c r="QM21">
+        <v>5.7176845468210079E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -31838,8 +32040,17 @@
       <c r="QJ22">
         <v>99.829861581495308</v>
       </c>
+      <c r="QK22" s="6">
+        <v>5154.2924999999996</v>
+      </c>
+      <c r="QL22" s="7">
+        <v>20454</v>
+      </c>
+      <c r="QM22">
+        <v>5.7176845468210079E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>377</v>
       </c>
@@ -33196,8 +33407,17 @@
       <c r="QJ23">
         <v>100.04370634025118</v>
       </c>
+      <c r="QK23" s="6">
+        <v>5154.2924999999996</v>
+      </c>
+      <c r="QL23" s="7">
+        <v>19898</v>
+      </c>
+      <c r="QM23">
+        <v>5.7176845468210079E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -34554,8 +34774,17 @@
       <c r="QJ24">
         <v>100.40011423587012</v>
       </c>
+      <c r="QK24" s="6">
+        <v>5154.2924999999996</v>
+      </c>
+      <c r="QL24" s="7">
+        <v>20499</v>
+      </c>
+      <c r="QM24">
+        <v>5.7176845468210079E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -35912,8 +36141,17 @@
       <c r="QJ25">
         <v>101.61190116651247</v>
       </c>
+      <c r="QK25" s="6">
+        <v>5065.8090000000002</v>
+      </c>
+      <c r="QL25" s="7">
+        <v>19044</v>
+      </c>
+      <c r="QM25">
+        <v>5.4935207953217643E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -37270,8 +37508,17 @@
       <c r="QJ26">
         <v>102.85932896156237</v>
       </c>
+      <c r="QK26" s="6">
+        <v>5065.8090000000002</v>
+      </c>
+      <c r="QL26" s="7">
+        <v>20039</v>
+      </c>
+      <c r="QM26">
+        <v>5.4935207953217643E-2</v>
+      </c>
     </row>
-    <row r="27" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>381</v>
       </c>
@@ -38628,8 +38875,17 @@
       <c r="QJ27">
         <v>102.75240658218445</v>
       </c>
+      <c r="QK27" s="6">
+        <v>5065.8090000000002</v>
+      </c>
+      <c r="QL27" s="7">
+        <v>20716</v>
+      </c>
+      <c r="QM27">
+        <v>5.4935207953217643E-2</v>
+      </c>
     </row>
-    <row r="28" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>382</v>
       </c>
@@ -39986,8 +40242,17 @@
       <c r="QJ28">
         <v>103.00189209842549</v>
       </c>
+      <c r="QK28" s="6">
+        <v>5065.8090000000002</v>
+      </c>
+      <c r="QL28" s="7">
+        <v>20558</v>
+      </c>
+      <c r="QM28">
+        <v>5.4935207953217643E-2</v>
+      </c>
     </row>
-    <row r="29" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -41344,8 +41609,17 @@
       <c r="QJ29">
         <v>104.35624227285329</v>
       </c>
+      <c r="QK29" s="6">
+        <v>5127.5469999999996</v>
+      </c>
+      <c r="QL29" s="7">
+        <v>19770</v>
+      </c>
+      <c r="QM29">
+        <v>5.4318242128429284E-2</v>
+      </c>
     </row>
-    <row r="30" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>384</v>
       </c>
@@ -42702,8 +42976,17 @@
       <c r="QJ30">
         <v>105.10469892849876</v>
       </c>
+      <c r="QK30" s="6">
+        <v>5127.5469999999996</v>
+      </c>
+      <c r="QL30" s="7">
+        <v>20983</v>
+      </c>
+      <c r="QM30">
+        <v>5.4318242128429284E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>385</v>
       </c>
@@ -44060,8 +44343,17 @@
       <c r="QJ31">
         <v>105.28290292976943</v>
       </c>
+      <c r="QK31" s="6">
+        <v>5127.5469999999996</v>
+      </c>
+      <c r="QL31" s="7">
+        <v>20461</v>
+      </c>
+      <c r="QM31">
+        <v>5.4318242128429284E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>386</v>
       </c>
@@ -45438,8 +45730,17 @@
       <c r="QJ32">
         <v>105.3185436872546</v>
       </c>
+      <c r="QK32" s="6">
+        <v>5127.5469999999996</v>
+      </c>
+      <c r="QL32" s="7">
+        <v>20834</v>
+      </c>
+      <c r="QM32">
+        <v>5.4318242128429284E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -46816,8 +47117,17 @@
       <c r="QJ33">
         <v>105.56802920349563</v>
       </c>
+      <c r="QK33" s="6">
+        <v>4565.9517500000002</v>
+      </c>
+      <c r="QL33" s="7">
+        <v>19760</v>
+      </c>
+      <c r="QM33">
+        <v>4.6055131075942349E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -48194,8 +48504,17 @@
       <c r="QJ34">
         <v>105.99571872100734</v>
       </c>
+      <c r="QK34" s="6">
+        <v>4565.9517500000002</v>
+      </c>
+      <c r="QL34" s="7">
+        <v>21611</v>
+      </c>
+      <c r="QM34">
+        <v>4.6055131075942349E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>389</v>
       </c>
@@ -49572,8 +49891,17 @@
       <c r="QJ35">
         <v>105.81751482665905</v>
       </c>
+      <c r="QK35" s="6">
+        <v>4565.9517500000002</v>
+      </c>
+      <c r="QL35" s="7">
+        <v>20216</v>
+      </c>
+      <c r="QM35">
+        <v>4.6055131075942349E-2</v>
+      </c>
     </row>
-    <row r="36" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -50950,8 +51278,17 @@
       <c r="QJ36">
         <v>105.99571872100734</v>
       </c>
+      <c r="QK36" s="6">
+        <v>4565.9517500000002</v>
+      </c>
+      <c r="QL36" s="7">
+        <v>21011</v>
+      </c>
+      <c r="QM36">
+        <v>4.6055131075942349E-2</v>
+      </c>
     </row>
-    <row r="37" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>391</v>
       </c>
@@ -52328,8 +52665,17 @@
       <c r="QJ37">
         <v>106.20956347976319</v>
       </c>
+      <c r="QK37" s="6">
+        <v>4094.8612499999999</v>
+      </c>
+      <c r="QL37" s="7">
+        <v>20466</v>
+      </c>
+      <c r="QM37">
+        <v>3.9418390577770933E-2</v>
+      </c>
     </row>
-    <row r="38" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>392</v>
       </c>
@@ -53706,8 +54052,17 @@
       <c r="QJ38">
         <v>106.63725299727486</v>
       </c>
+      <c r="QK38" s="6">
+        <v>4094.8612499999999</v>
+      </c>
+      <c r="QL38" s="7">
+        <v>21954</v>
+      </c>
+      <c r="QM38">
+        <v>3.9418390577770933E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>393</v>
       </c>
@@ -55084,8 +55439,17 @@
       <c r="QJ39">
         <v>106.42340823851902</v>
       </c>
+      <c r="QK39" s="6">
+        <v>4094.8612499999999</v>
+      </c>
+      <c r="QL39" s="7">
+        <v>20407</v>
+      </c>
+      <c r="QM39">
+        <v>3.9418390577770933E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>394</v>
       </c>
@@ -56462,8 +56826,17 @@
       <c r="QJ40">
         <v>106.49468986041177</v>
       </c>
+      <c r="QK40" s="6">
+        <v>4094.8612499999999</v>
+      </c>
+      <c r="QL40" s="7">
+        <v>21879</v>
+      </c>
+      <c r="QM40">
+        <v>3.9418390577770933E-2</v>
+      </c>
     </row>
-    <row r="41" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -57840,8 +58213,17 @@
       <c r="QJ41">
         <v>106.49468986041177</v>
       </c>
+      <c r="QK41" s="6">
+        <v>3891.779</v>
+      </c>
+      <c r="QL41" s="7">
+        <v>20713</v>
+      </c>
+      <c r="QM41">
+        <v>3.7532828623782426E-2</v>
+      </c>
     </row>
-    <row r="42" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>396</v>
       </c>
@@ -59218,8 +59600,17 @@
       <c r="QJ42">
         <v>107.27878695277528</v>
       </c>
+      <c r="QK42" s="6">
+        <v>3891.779</v>
+      </c>
+      <c r="QL42" s="7">
+        <v>22645</v>
+      </c>
+      <c r="QM42">
+        <v>3.7532828623782426E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>397</v>
       </c>
@@ -60596,8 +60987,17 @@
       <c r="QJ43">
         <v>107.06494219401941</v>
       </c>
+      <c r="QK43" s="6">
+        <v>3891.779</v>
+      </c>
+      <c r="QL43" s="7">
+        <v>21102</v>
+      </c>
+      <c r="QM43">
+        <v>3.7532828623782426E-2</v>
+      </c>
     </row>
-    <row r="44" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>398</v>
       </c>
@@ -61974,8 +62374,17 @@
       <c r="QJ44">
         <v>106.85109775603071</v>
       </c>
+      <c r="QK44" s="6">
+        <v>3891.779</v>
+      </c>
+      <c r="QL44" s="7">
+        <v>22898</v>
+      </c>
+      <c r="QM44">
+        <v>3.7532828623782426E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>399</v>
       </c>
@@ -63352,8 +63761,17 @@
       <c r="QJ45">
         <v>106.81545699854553</v>
       </c>
+      <c r="QK45" s="6">
+        <v>3644.1424999999999</v>
+      </c>
+      <c r="QL45" s="7">
+        <v>21324</v>
+      </c>
+      <c r="QM45">
+        <v>3.5174950893094144E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>400</v>
       </c>
@@ -64730,8 +65148,17 @@
       <c r="QJ46">
         <v>107.42135083809502</v>
       </c>
+      <c r="QK46" s="6">
+        <v>3644.1424999999999</v>
+      </c>
+      <c r="QL46" s="7">
+        <v>23314</v>
+      </c>
+      <c r="QM46">
+        <v>3.5174950893094144E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>401</v>
       </c>
@@ -66108,8 +66535,17 @@
       <c r="QJ47">
         <v>107.24314651605722</v>
       </c>
+      <c r="QK47" s="6">
+        <v>3644.1424999999999</v>
+      </c>
+      <c r="QL47" s="7">
+        <v>22001</v>
+      </c>
+      <c r="QM47">
+        <v>3.5174950893094144E-2</v>
+      </c>
     </row>
-    <row r="48" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -67486,8 +67922,17 @@
       <c r="QJ48">
         <v>107.27878695277528</v>
       </c>
+      <c r="QK48" s="6">
+        <v>3644.1424999999999</v>
+      </c>
+      <c r="QL48" s="7">
+        <v>23689</v>
+      </c>
+      <c r="QM48">
+        <v>3.5174950893094144E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>403</v>
       </c>
@@ -68864,8 +69309,17 @@
       <c r="QJ49">
         <v>107.84904035560675</v>
       </c>
+      <c r="QK49" s="6">
+        <v>3771.1925000000001</v>
+      </c>
+      <c r="QL49" s="7">
+        <v>22201</v>
+      </c>
+      <c r="QM49">
+        <v>3.5915178411993973E-2</v>
+      </c>
     </row>
-    <row r="50" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>404</v>
       </c>
@@ -70242,8 +70696,17 @@
       <c r="QJ50">
         <v>108.31237030983647</v>
       </c>
+      <c r="QK50" s="6">
+        <v>3771.1925000000001</v>
+      </c>
+      <c r="QL50" s="7">
+        <v>24527</v>
+      </c>
+      <c r="QM50">
+        <v>3.5915178411993973E-2</v>
+      </c>
     </row>
-    <row r="51" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -71620,8 +72083,17 @@
       <c r="QJ51">
         <v>108.88262264344412</v>
       </c>
+      <c r="QK51" s="6">
+        <v>3771.1925000000001</v>
+      </c>
+      <c r="QL51" s="7">
+        <v>22701</v>
+      </c>
+      <c r="QM51">
+        <v>3.5915178411993973E-2</v>
+      </c>
     </row>
-    <row r="52" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>406</v>
       </c>
@@ -72998,8 +73470,17 @@
       <c r="QJ52">
         <v>108.63313744797023</v>
       </c>
+      <c r="QK52" s="6">
+        <v>3771.1925000000001</v>
+      </c>
+      <c r="QL52" s="7">
+        <v>24820</v>
+      </c>
+      <c r="QM52">
+        <v>3.5915178411993973E-2</v>
+      </c>
     </row>
-    <row r="53" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>407</v>
       </c>
@@ -74376,8 +74857,17 @@
       <c r="QJ53">
         <v>108.49057463187427</v>
       </c>
+      <c r="QK53" s="6">
+        <v>3605.89075</v>
+      </c>
+      <c r="QL53" s="7">
+        <v>22973</v>
+      </c>
+      <c r="QM53">
+        <v>3.3921433191049025E-2</v>
+      </c>
     </row>
-    <row r="54" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -75755,8 +76245,17 @@
       <c r="QJ54">
         <v>109.3815941036157</v>
       </c>
+      <c r="QK54" s="6">
+        <v>3605.89075</v>
+      </c>
+      <c r="QL54" s="7">
+        <v>25673</v>
+      </c>
+      <c r="QM54">
+        <v>3.3921433191049025E-2</v>
+      </c>
     </row>
-    <row r="55" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -77134,8 +77633,17 @@
       <c r="QJ55">
         <v>109.84492405784543</v>
       </c>
+      <c r="QK55" s="6">
+        <v>3605.89075</v>
+      </c>
+      <c r="QL55" s="7">
+        <v>23584</v>
+      </c>
+      <c r="QM55">
+        <v>3.3921433191049025E-2</v>
+      </c>
     </row>
-    <row r="56" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>410</v>
       </c>
@@ -78513,8 +79021,17 @@
       <c r="QJ56">
         <v>109.48851648299362</v>
       </c>
+      <c r="QK56" s="6">
+        <v>3605.89075</v>
+      </c>
+      <c r="QL56" s="7">
+        <v>26095</v>
+      </c>
+      <c r="QM56">
+        <v>3.3921433191049025E-2</v>
+      </c>
     </row>
-    <row r="57" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>411</v>
       </c>
@@ -79892,8 +80409,17 @@
       <c r="QJ57">
         <v>109.77364318440935</v>
       </c>
+      <c r="QK57" s="6">
+        <v>3762.6637500000002</v>
+      </c>
+      <c r="QL57" s="7">
+        <v>23884</v>
+      </c>
+      <c r="QM57">
+        <v>3.438687780737789E-2</v>
+      </c>
     </row>
-    <row r="58" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>412</v>
       </c>
@@ -81271,8 +81797,17 @@
       <c r="QJ58">
         <v>110.20133270192103</v>
       </c>
+      <c r="QK58" s="6">
+        <v>3762.6637500000002</v>
+      </c>
+      <c r="QL58" s="7">
+        <v>26283</v>
+      </c>
+      <c r="QM58">
+        <v>3.438687780737789E-2</v>
+      </c>
     </row>
-    <row r="59" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>413</v>
       </c>
@@ -82650,8 +83185,17 @@
       <c r="QJ59">
         <v>110.30825508129897</v>
       </c>
+      <c r="QK59" s="6">
+        <v>3762.6637500000002</v>
+      </c>
+      <c r="QL59" s="7">
+        <v>24325</v>
+      </c>
+      <c r="QM59">
+        <v>3.438687780737789E-2</v>
+      </c>
     </row>
-    <row r="60" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>414</v>
       </c>
@@ -84029,8 +84573,17 @@
       <c r="QJ60">
         <v>110.23697313863909</v>
       </c>
+      <c r="QK60" s="6">
+        <v>3762.6637500000002</v>
+      </c>
+      <c r="QL60" s="7">
+        <v>26321</v>
+      </c>
+      <c r="QM60">
+        <v>3.438687780737789E-2</v>
+      </c>
     </row>
-    <row r="61" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>415</v>
       </c>
@@ -85408,8 +85961,17 @@
       <c r="QJ61">
         <v>110.45081789739493</v>
       </c>
+      <c r="QK61" s="6">
+        <v>5366.1265000000003</v>
+      </c>
+      <c r="QL61" s="7">
+        <v>24357</v>
+      </c>
+      <c r="QM61">
+        <v>4.675629530879688E-2</v>
+      </c>
     </row>
-    <row r="62" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF62" s="1"/>
       <c r="LG62" s="1"/>
       <c r="LH62" s="1"/>
@@ -85453,8 +86015,9 @@
       <c r="MT62" s="1"/>
       <c r="MU62" s="1"/>
       <c r="QF62" s="5"/>
+      <c r="QK62" s="6"/>
     </row>
-    <row r="63" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF63" s="1"/>
       <c r="LG63" s="1"/>
       <c r="LH63" s="1"/>
@@ -85498,8 +86061,9 @@
       <c r="MT63" s="1"/>
       <c r="MU63" s="1"/>
       <c r="QF63" s="5"/>
+      <c r="QK63" s="6"/>
     </row>
-    <row r="64" spans="1:452" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:455" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF64" s="1"/>
       <c r="LG64" s="1"/>
       <c r="LH64" s="1"/>
@@ -85543,22 +86107,25 @@
       <c r="MT64" s="1"/>
       <c r="MU64" s="1"/>
       <c r="QF64" s="5"/>
+      <c r="QK64" s="6"/>
     </row>
-    <row r="65" spans="448:448" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="448:453" ht="15.75" x14ac:dyDescent="0.25">
       <c r="QF65" s="5"/>
+      <c r="QK65" s="6"/>
     </row>
-    <row r="66" spans="448:448" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="448:453" ht="15.75" x14ac:dyDescent="0.25">
       <c r="QF66" s="5"/>
     </row>
-    <row r="67" spans="448:448" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="448:453" ht="15.75" x14ac:dyDescent="0.25">
       <c r="QF67" s="5"/>
     </row>
-    <row r="68" spans="448:448" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="448:453" ht="15.75" x14ac:dyDescent="0.25">
       <c r="QF68" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -85568,7 +86135,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nyt dataset + opdateringer til model
</commit_message>
<xml_diff>
--- a/AAMK.xlsx
+++ b/AAMK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon ik mig\Desktop\9. Semester\Arbejdsmarkeds projekt\Empirisk-SFC-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7D813F-8097-4DCD-8791-481A5757C2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF15935-6F3C-429F-861F-3F1A1F892DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="524">
   <si>
     <t>IBA_h</t>
   </si>
@@ -1590,15 +1590,37 @@
   <si>
     <t>emp_ratio</t>
   </si>
+  <si>
+    <t>tyd</t>
+  </si>
+  <si>
+    <t>uld</t>
+  </si>
+  <si>
+    <t>kuld</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>tydd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1657,25 +1679,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{9E53180C-48BC-4FF6-AB51-113B5820BC5D}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{9D0EE842-C58A-4ACA-83D6-D8F46096A387}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1987,11 +2014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:QQ68"/>
+  <dimension ref="A1:QV68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="QH2" sqref="QH2"/>
+      <pane xSplit="1" topLeftCell="QK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="QW2" sqref="QW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +2026,7 @@
     <col min="456" max="456" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>496</v>
       </c>
@@ -3377,8 +3404,23 @@
       <c r="QQ1" t="s">
         <v>517</v>
       </c>
+      <c r="QR1" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="QS1" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="QT1" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="QU1" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="QV1" s="10" t="s">
+        <v>523</v>
+      </c>
     </row>
-    <row r="2" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -4757,8 +4799,23 @@
       <c r="QQ2">
         <v>7.2398729939877629E-2</v>
       </c>
+      <c r="QR2" s="8">
+        <v>19029</v>
+      </c>
+      <c r="QS2" s="8">
+        <v>117.098</v>
+      </c>
+      <c r="QT2" s="8">
+        <v>0.82888915630242588</v>
+      </c>
+      <c r="QU2" s="8">
+        <v>141.27099999999999</v>
+      </c>
+      <c r="QV2" s="10">
+        <v>19029</v>
+      </c>
     </row>
-    <row r="3" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>357</v>
       </c>
@@ -6137,8 +6194,23 @@
       <c r="QQ3">
         <v>7.2398729939877629E-2</v>
       </c>
+      <c r="QR3" s="8">
+        <v>19029</v>
+      </c>
+      <c r="QS3" s="8">
+        <v>117.098</v>
+      </c>
+      <c r="QT3" s="8">
+        <v>0.82888915630242588</v>
+      </c>
+      <c r="QU3" s="8">
+        <v>141.27099999999999</v>
+      </c>
+      <c r="QV3" s="10">
+        <v>19029</v>
+      </c>
     </row>
-    <row r="4" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -7517,8 +7589,23 @@
       <c r="QQ4">
         <v>7.2398729939877629E-2</v>
       </c>
+      <c r="QR4" s="8">
+        <v>19029</v>
+      </c>
+      <c r="QS4" s="8">
+        <v>117.098</v>
+      </c>
+      <c r="QT4" s="8">
+        <v>0.82888915630242588</v>
+      </c>
+      <c r="QU4" s="8">
+        <v>141.27099999999999</v>
+      </c>
+      <c r="QV4" s="10">
+        <v>19029</v>
+      </c>
     </row>
-    <row r="5" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -8897,8 +8984,23 @@
       <c r="QQ5">
         <v>5.5094098133709461E-2</v>
       </c>
+      <c r="QR5" s="8">
+        <v>14617</v>
+      </c>
+      <c r="QS5" s="8">
+        <v>87.972999999999999</v>
+      </c>
+      <c r="QT5" s="8">
+        <v>0.80514904404967824</v>
+      </c>
+      <c r="QU5" s="8">
+        <v>109.26300000000001</v>
+      </c>
+      <c r="QV5" s="10">
+        <v>14617</v>
+      </c>
     </row>
-    <row r="6" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -10277,8 +10379,23 @@
       <c r="QQ6">
         <v>5.5094098133709461E-2</v>
       </c>
+      <c r="QR6" s="8">
+        <v>14617</v>
+      </c>
+      <c r="QS6" s="8">
+        <v>87.972999999999999</v>
+      </c>
+      <c r="QT6" s="8">
+        <v>0.80514904404967824</v>
+      </c>
+      <c r="QU6" s="8">
+        <v>109.26300000000001</v>
+      </c>
+      <c r="QV6" s="10">
+        <v>14617</v>
+      </c>
     </row>
-    <row r="7" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -11657,8 +11774,23 @@
       <c r="QQ7">
         <v>5.5094098133709461E-2</v>
       </c>
+      <c r="QR7" s="8">
+        <v>14617</v>
+      </c>
+      <c r="QS7" s="8">
+        <v>87.972999999999999</v>
+      </c>
+      <c r="QT7" s="8">
+        <v>0.80514904404967824</v>
+      </c>
+      <c r="QU7" s="8">
+        <v>109.26300000000001</v>
+      </c>
+      <c r="QV7" s="10">
+        <v>14617</v>
+      </c>
     </row>
-    <row r="8" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -13037,8 +13169,23 @@
       <c r="QQ8">
         <v>5.5094098133709461E-2</v>
       </c>
+      <c r="QR8" s="8">
+        <v>14617</v>
+      </c>
+      <c r="QS8" s="8">
+        <v>87.972999999999999</v>
+      </c>
+      <c r="QT8" s="8">
+        <v>0.80514904404967824</v>
+      </c>
+      <c r="QU8" s="8">
+        <v>109.26300000000001</v>
+      </c>
+      <c r="QV8" s="10">
+        <v>14617</v>
+      </c>
     </row>
-    <row r="9" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>363</v>
       </c>
@@ -14417,8 +14564,23 @@
       <c r="QQ9">
         <v>3.8281381416352886E-2</v>
       </c>
+      <c r="QR9" s="8">
+        <v>10407</v>
+      </c>
+      <c r="QS9" s="8">
+        <v>60.328050000000005</v>
+      </c>
+      <c r="QT9" s="8">
+        <v>0.7899092864674464</v>
+      </c>
+      <c r="QU9" s="8">
+        <v>76.373390000000001</v>
+      </c>
+      <c r="QV9" s="10">
+        <v>10407</v>
+      </c>
     </row>
-    <row r="10" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -15797,8 +15959,23 @@
       <c r="QQ10">
         <v>3.8281381416352886E-2</v>
       </c>
+      <c r="QR10" s="8">
+        <v>10407</v>
+      </c>
+      <c r="QS10" s="8">
+        <v>60.328050000000005</v>
+      </c>
+      <c r="QT10" s="8">
+        <v>0.7899092864674464</v>
+      </c>
+      <c r="QU10" s="8">
+        <v>76.373390000000001</v>
+      </c>
+      <c r="QV10" s="10">
+        <v>10407</v>
+      </c>
     </row>
-    <row r="11" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>365</v>
       </c>
@@ -17177,8 +17354,23 @@
       <c r="QQ11">
         <v>3.8281381416352886E-2</v>
       </c>
+      <c r="QR11" s="8">
+        <v>10407</v>
+      </c>
+      <c r="QS11" s="8">
+        <v>60.328050000000005</v>
+      </c>
+      <c r="QT11" s="8">
+        <v>0.7899092864674464</v>
+      </c>
+      <c r="QU11" s="8">
+        <v>76.373390000000001</v>
+      </c>
+      <c r="QV11" s="10">
+        <v>10407</v>
+      </c>
     </row>
-    <row r="12" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -18557,8 +18749,23 @@
       <c r="QQ12">
         <v>3.8281381416352886E-2</v>
       </c>
+      <c r="QR12" s="8">
+        <v>10407</v>
+      </c>
+      <c r="QS12" s="8">
+        <v>60.328050000000005</v>
+      </c>
+      <c r="QT12" s="8">
+        <v>0.7899092864674464</v>
+      </c>
+      <c r="QU12" s="8">
+        <v>76.373390000000001</v>
+      </c>
+      <c r="QV12" s="10">
+        <v>10407</v>
+      </c>
     </row>
-    <row r="13" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>367</v>
       </c>
@@ -19937,8 +20144,23 @@
       <c r="QQ13">
         <v>2.6161771362630776E-2</v>
       </c>
+      <c r="QR13" s="8">
+        <v>6955</v>
+      </c>
+      <c r="QS13" s="8">
+        <v>39.656680000000001</v>
+      </c>
+      <c r="QT13" s="8">
+        <v>0.77740940638274025</v>
+      </c>
+      <c r="QU13" s="8">
+        <v>51.011319999999998</v>
+      </c>
+      <c r="QV13" s="10">
+        <v>6955</v>
+      </c>
     </row>
-    <row r="14" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -21317,8 +21539,23 @@
       <c r="QQ14">
         <v>2.6161771362630776E-2</v>
       </c>
+      <c r="QR14" s="8">
+        <v>6955</v>
+      </c>
+      <c r="QS14" s="8">
+        <v>39.656680000000001</v>
+      </c>
+      <c r="QT14" s="8">
+        <v>0.77740940638274025</v>
+      </c>
+      <c r="QU14" s="8">
+        <v>51.011319999999998</v>
+      </c>
+      <c r="QV14" s="10">
+        <v>6955</v>
+      </c>
     </row>
-    <row r="15" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>369</v>
       </c>
@@ -22697,8 +22934,23 @@
       <c r="QQ15">
         <v>2.6161771362630776E-2</v>
       </c>
+      <c r="QR15" s="8">
+        <v>6955</v>
+      </c>
+      <c r="QS15" s="8">
+        <v>39.656680000000001</v>
+      </c>
+      <c r="QT15" s="8">
+        <v>0.77740940638274025</v>
+      </c>
+      <c r="QU15" s="8">
+        <v>51.011319999999998</v>
+      </c>
+      <c r="QV15" s="10">
+        <v>6955</v>
+      </c>
     </row>
-    <row r="16" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>370</v>
       </c>
@@ -24077,8 +24329,23 @@
       <c r="QQ16">
         <v>2.6161771362630776E-2</v>
       </c>
+      <c r="QR16" s="8">
+        <v>6955</v>
+      </c>
+      <c r="QS16" s="8">
+        <v>39.656680000000001</v>
+      </c>
+      <c r="QT16" s="8">
+        <v>0.77740940638274025</v>
+      </c>
+      <c r="QU16" s="8">
+        <v>51.011319999999998</v>
+      </c>
+      <c r="QV16" s="10">
+        <v>6955</v>
+      </c>
     </row>
-    <row r="17" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>371</v>
       </c>
@@ -25457,8 +25724,23 @@
       <c r="QQ17">
         <v>4.8197032814441279E-2</v>
       </c>
+      <c r="QR17" s="8">
+        <v>14571</v>
+      </c>
+      <c r="QS17" s="8">
+        <v>84.384479999999996</v>
+      </c>
+      <c r="QT17" s="8">
+        <v>0.84858294774704035</v>
+      </c>
+      <c r="QU17" s="8">
+        <v>99.441639999999992</v>
+      </c>
+      <c r="QV17" s="10">
+        <v>14571</v>
+      </c>
     </row>
-    <row r="18" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -26837,8 +27119,23 @@
       <c r="QQ18">
         <v>4.8197032814441279E-2</v>
       </c>
+      <c r="QR18" s="8">
+        <v>14571</v>
+      </c>
+      <c r="QS18" s="8">
+        <v>84.384479999999996</v>
+      </c>
+      <c r="QT18" s="8">
+        <v>0.84858294774704035</v>
+      </c>
+      <c r="QU18" s="8">
+        <v>99.441639999999992</v>
+      </c>
+      <c r="QV18" s="10">
+        <v>14571</v>
+      </c>
     </row>
-    <row r="19" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>373</v>
       </c>
@@ -28217,8 +28514,23 @@
       <c r="QQ19">
         <v>4.8197032814441279E-2</v>
       </c>
+      <c r="QR19" s="8">
+        <v>14571</v>
+      </c>
+      <c r="QS19" s="8">
+        <v>84.384479999999996</v>
+      </c>
+      <c r="QT19" s="8">
+        <v>0.84858294774704035</v>
+      </c>
+      <c r="QU19" s="8">
+        <v>99.441639999999992</v>
+      </c>
+      <c r="QV19" s="10">
+        <v>14571</v>
+      </c>
     </row>
-    <row r="20" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>374</v>
       </c>
@@ -29597,8 +29909,23 @@
       <c r="QQ20">
         <v>4.8197032814441279E-2</v>
       </c>
+      <c r="QR20" s="8">
+        <v>14571</v>
+      </c>
+      <c r="QS20" s="8">
+        <v>84.384479999999996</v>
+      </c>
+      <c r="QT20" s="8">
+        <v>0.84858294774704035</v>
+      </c>
+      <c r="QU20" s="8">
+        <v>99.441639999999992</v>
+      </c>
+      <c r="QV20" s="10">
+        <v>14571</v>
+      </c>
     </row>
-    <row r="21" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>375</v>
       </c>
@@ -30977,8 +31304,23 @@
       <c r="QQ21">
         <v>6.0110486818678484E-2</v>
       </c>
+      <c r="QR21" s="8">
+        <v>18082.780340742898</v>
+      </c>
+      <c r="QS21" s="8">
+        <v>96.056440000000009</v>
+      </c>
+      <c r="QT21" s="8">
+        <v>0.84593139124147632</v>
+      </c>
+      <c r="QU21" s="8">
+        <v>113.55110000000001</v>
+      </c>
+      <c r="QV21" s="10">
+        <v>18082.780340742898</v>
+      </c>
     </row>
-    <row r="22" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -32357,8 +32699,23 @@
       <c r="QQ22">
         <v>6.0110486818678484E-2</v>
       </c>
+      <c r="QR22" s="8">
+        <v>18082.780340742898</v>
+      </c>
+      <c r="QS22" s="8">
+        <v>96.056440000000009</v>
+      </c>
+      <c r="QT22" s="8">
+        <v>0.84593139124147632</v>
+      </c>
+      <c r="QU22" s="8">
+        <v>113.55110000000001</v>
+      </c>
+      <c r="QV22" s="10">
+        <v>18082.780340742898</v>
+      </c>
     </row>
-    <row r="23" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>377</v>
       </c>
@@ -33737,8 +34094,23 @@
       <c r="QQ23">
         <v>6.0110486818678484E-2</v>
       </c>
+      <c r="QR23" s="8">
+        <v>18082.780340742898</v>
+      </c>
+      <c r="QS23" s="8">
+        <v>96.056440000000009</v>
+      </c>
+      <c r="QT23" s="8">
+        <v>0.84593139124147632</v>
+      </c>
+      <c r="QU23" s="8">
+        <v>113.55110000000001</v>
+      </c>
+      <c r="QV23" s="10">
+        <v>18082.780340742898</v>
+      </c>
     </row>
-    <row r="24" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -35117,8 +35489,23 @@
       <c r="QQ24">
         <v>6.0110486818678484E-2</v>
       </c>
+      <c r="QR24" s="8">
+        <v>18082.780340742898</v>
+      </c>
+      <c r="QS24" s="8">
+        <v>96.056440000000009</v>
+      </c>
+      <c r="QT24" s="8">
+        <v>0.84593139124147632</v>
+      </c>
+      <c r="QU24" s="8">
+        <v>113.55110000000001</v>
+      </c>
+      <c r="QV24" s="10">
+        <v>18082.780340742898</v>
+      </c>
     </row>
-    <row r="25" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -36497,8 +36884,23 @@
       <c r="QQ25">
         <v>5.6970587517655893E-2</v>
       </c>
+      <c r="QR25" s="8">
+        <v>17011.423221768997</v>
+      </c>
+      <c r="QS25" s="8">
+        <v>89.218050000000005</v>
+      </c>
+      <c r="QT25" s="8">
+        <v>0.82554116599828642</v>
+      </c>
+      <c r="QU25" s="8">
+        <v>108.0722</v>
+      </c>
+      <c r="QV25" s="10">
+        <v>17011.423221768997</v>
+      </c>
     </row>
-    <row r="26" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -37877,8 +38279,23 @@
       <c r="QQ26">
         <v>5.6970587517655893E-2</v>
       </c>
+      <c r="QR26" s="8">
+        <v>17011.423221768997</v>
+      </c>
+      <c r="QS26" s="8">
+        <v>89.218050000000005</v>
+      </c>
+      <c r="QT26" s="8">
+        <v>0.82554116599828642</v>
+      </c>
+      <c r="QU26" s="8">
+        <v>108.0722</v>
+      </c>
+      <c r="QV26" s="10">
+        <v>17011.423221768997</v>
+      </c>
     </row>
-    <row r="27" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>381</v>
       </c>
@@ -39257,8 +39674,23 @@
       <c r="QQ27">
         <v>5.6970587517655893E-2</v>
       </c>
+      <c r="QR27" s="8">
+        <v>17011.423221768997</v>
+      </c>
+      <c r="QS27" s="8">
+        <v>89.218050000000005</v>
+      </c>
+      <c r="QT27" s="8">
+        <v>0.82554116599828642</v>
+      </c>
+      <c r="QU27" s="8">
+        <v>108.0722</v>
+      </c>
+      <c r="QV27" s="10">
+        <v>17011.423221768997</v>
+      </c>
     </row>
-    <row r="28" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>382</v>
       </c>
@@ -40637,8 +41069,23 @@
       <c r="QQ28">
         <v>5.6970587517655893E-2</v>
       </c>
+      <c r="QR28" s="8">
+        <v>17011.423221768997</v>
+      </c>
+      <c r="QS28" s="8">
+        <v>89.218050000000005</v>
+      </c>
+      <c r="QT28" s="8">
+        <v>0.82554116599828642</v>
+      </c>
+      <c r="QU28" s="8">
+        <v>108.0722</v>
+      </c>
+      <c r="QV28" s="10">
+        <v>17011.423221768997</v>
+      </c>
     </row>
-    <row r="29" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -42017,8 +42464,23 @@
       <c r="QQ29">
         <v>5.8602781301560145E-2</v>
       </c>
+      <c r="QR29" s="8">
+        <v>18883.449153889494</v>
+      </c>
+      <c r="QS29" s="8">
+        <v>98.564880000000002</v>
+      </c>
+      <c r="QT29" s="8">
+        <v>0.82661404419516049</v>
+      </c>
+      <c r="QU29" s="8">
+        <v>119.2393</v>
+      </c>
+      <c r="QV29" s="10">
+        <v>18883.449153889494</v>
+      </c>
     </row>
-    <row r="30" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>384</v>
       </c>
@@ -43397,8 +43859,23 @@
       <c r="QQ30">
         <v>5.8602781301560145E-2</v>
       </c>
+      <c r="QR30" s="8">
+        <v>18883.449153889494</v>
+      </c>
+      <c r="QS30" s="8">
+        <v>98.564880000000002</v>
+      </c>
+      <c r="QT30" s="8">
+        <v>0.82661404419516049</v>
+      </c>
+      <c r="QU30" s="8">
+        <v>119.2393</v>
+      </c>
+      <c r="QV30" s="10">
+        <v>18883.449153889494</v>
+      </c>
     </row>
-    <row r="31" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>385</v>
       </c>
@@ -44777,8 +45254,23 @@
       <c r="QQ31">
         <v>5.8602781301560145E-2</v>
       </c>
+      <c r="QR31" s="8">
+        <v>18883.449153889494</v>
+      </c>
+      <c r="QS31" s="8">
+        <v>98.564880000000002</v>
+      </c>
+      <c r="QT31" s="8">
+        <v>0.82661404419516049</v>
+      </c>
+      <c r="QU31" s="8">
+        <v>119.2393</v>
+      </c>
+      <c r="QV31" s="10">
+        <v>18883.449153889494</v>
+      </c>
     </row>
-    <row r="32" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>386</v>
       </c>
@@ -46177,8 +46669,23 @@
       <c r="QQ32">
         <v>5.8602781301560145E-2</v>
       </c>
+      <c r="QR32" s="8">
+        <v>18883.449153889494</v>
+      </c>
+      <c r="QS32" s="8">
+        <v>98.564880000000002</v>
+      </c>
+      <c r="QT32" s="8">
+        <v>0.82661404419516049</v>
+      </c>
+      <c r="QU32" s="8">
+        <v>119.2393</v>
+      </c>
+      <c r="QV32" s="10">
+        <v>18883.449153889494</v>
+      </c>
     </row>
-    <row r="33" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -47577,8 +48084,23 @@
       <c r="QQ33">
         <v>4.9754894544134114E-2</v>
       </c>
+      <c r="QR33" s="8">
+        <v>17305.191954202463</v>
+      </c>
+      <c r="QS33" s="8">
+        <v>87.008630000000011</v>
+      </c>
+      <c r="QT33" s="8">
+        <v>0.7418608458250594</v>
+      </c>
+      <c r="QU33" s="8">
+        <v>117.2843</v>
+      </c>
+      <c r="QV33" s="10">
+        <v>17305.191954202463</v>
+      </c>
     </row>
-    <row r="34" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -48977,8 +49499,23 @@
       <c r="QQ34">
         <v>4.9754894544134114E-2</v>
       </c>
+      <c r="QR34" s="8">
+        <v>17305.191954202463</v>
+      </c>
+      <c r="QS34" s="8">
+        <v>87.008630000000011</v>
+      </c>
+      <c r="QT34" s="8">
+        <v>0.7418608458250594</v>
+      </c>
+      <c r="QU34" s="8">
+        <v>117.2843</v>
+      </c>
+      <c r="QV34" s="10">
+        <v>17305.191954202463</v>
+      </c>
     </row>
-    <row r="35" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>389</v>
       </c>
@@ -50377,8 +50914,23 @@
       <c r="QQ35">
         <v>4.9754894544134114E-2</v>
       </c>
+      <c r="QR35" s="8">
+        <v>17305.191954202463</v>
+      </c>
+      <c r="QS35" s="8">
+        <v>87.008630000000011</v>
+      </c>
+      <c r="QT35" s="8">
+        <v>0.7418608458250594</v>
+      </c>
+      <c r="QU35" s="8">
+        <v>117.2843</v>
+      </c>
+      <c r="QV35" s="10">
+        <v>17305.191954202463</v>
+      </c>
     </row>
-    <row r="36" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -51777,8 +52329,23 @@
       <c r="QQ36">
         <v>4.9754894544134114E-2</v>
       </c>
+      <c r="QR36" s="8">
+        <v>17305.191954202463</v>
+      </c>
+      <c r="QS36" s="8">
+        <v>87.008630000000011</v>
+      </c>
+      <c r="QT36" s="8">
+        <v>0.7418608458250594</v>
+      </c>
+      <c r="QU36" s="8">
+        <v>117.2843</v>
+      </c>
+      <c r="QV36" s="10">
+        <v>17305.191954202463</v>
+      </c>
     </row>
-    <row r="37" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>391</v>
       </c>
@@ -53177,8 +53744,23 @@
       <c r="QQ37">
         <v>4.4885061897152537E-2</v>
       </c>
+      <c r="QR37" s="8">
+        <v>16478.796438511527</v>
+      </c>
+      <c r="QS37" s="8">
+        <v>84.32535</v>
+      </c>
+      <c r="QT37" s="8">
+        <v>0.79342558014153164</v>
+      </c>
+      <c r="QU37" s="8">
+        <v>106.2801</v>
+      </c>
+      <c r="QV37" s="10">
+        <v>15672.358399246803</v>
+      </c>
     </row>
-    <row r="38" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>392</v>
       </c>
@@ -54577,8 +55159,23 @@
       <c r="QQ38">
         <v>4.4885061897152537E-2</v>
       </c>
+      <c r="QR38" s="8">
+        <v>16478.796438511527</v>
+      </c>
+      <c r="QS38" s="8">
+        <v>84.32535</v>
+      </c>
+      <c r="QT38" s="8">
+        <v>0.79342558014153164</v>
+      </c>
+      <c r="QU38" s="8">
+        <v>106.2801</v>
+      </c>
+      <c r="QV38" s="10">
+        <v>15672.358399246803</v>
+      </c>
     </row>
-    <row r="39" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>393</v>
       </c>
@@ -55977,8 +56574,23 @@
       <c r="QQ39">
         <v>4.4885061897152537E-2</v>
       </c>
+      <c r="QR39" s="8">
+        <v>16478.796438511527</v>
+      </c>
+      <c r="QS39" s="8">
+        <v>84.32535</v>
+      </c>
+      <c r="QT39" s="8">
+        <v>0.79342558014153164</v>
+      </c>
+      <c r="QU39" s="8">
+        <v>106.2801</v>
+      </c>
+      <c r="QV39" s="10">
+        <v>15672.358399246803</v>
+      </c>
     </row>
-    <row r="40" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>394</v>
       </c>
@@ -57377,8 +57989,23 @@
       <c r="QQ40">
         <v>4.4885061897152537E-2</v>
       </c>
+      <c r="QR40" s="8">
+        <v>16478.796438511527</v>
+      </c>
+      <c r="QS40" s="8">
+        <v>84.32535</v>
+      </c>
+      <c r="QT40" s="8">
+        <v>0.79342558014153164</v>
+      </c>
+      <c r="QU40" s="8">
+        <v>106.2801</v>
+      </c>
+      <c r="QV40" s="10">
+        <v>15672.358399246803</v>
+      </c>
     </row>
-    <row r="41" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -58777,8 +59404,23 @@
       <c r="QQ41">
         <v>4.3745780692448645E-2</v>
       </c>
+      <c r="QR41" s="8">
+        <v>16377.960176766268</v>
+      </c>
+      <c r="QS41" s="8">
+        <v>83.144990000000007</v>
+      </c>
+      <c r="QT41" s="8">
+        <v>0.81786596420059243</v>
+      </c>
+      <c r="QU41" s="8">
+        <v>101.6609</v>
+      </c>
+      <c r="QV41" s="10">
+        <v>15239.509383760982</v>
+      </c>
     </row>
-    <row r="42" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>396</v>
       </c>
@@ -60177,8 +60819,23 @@
       <c r="QQ42">
         <v>4.3745780692448645E-2</v>
       </c>
+      <c r="QR42" s="8">
+        <v>16377.960176766268</v>
+      </c>
+      <c r="QS42" s="8">
+        <v>83.144990000000007</v>
+      </c>
+      <c r="QT42" s="8">
+        <v>0.81786596420059243</v>
+      </c>
+      <c r="QU42" s="8">
+        <v>101.6609</v>
+      </c>
+      <c r="QV42" s="10">
+        <v>15239.509383760982</v>
+      </c>
     </row>
-    <row r="43" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>397</v>
       </c>
@@ -61577,8 +62234,23 @@
       <c r="QQ43">
         <v>4.3745780692448645E-2</v>
       </c>
+      <c r="QR43" s="8">
+        <v>16377.960176766268</v>
+      </c>
+      <c r="QS43" s="8">
+        <v>83.144990000000007</v>
+      </c>
+      <c r="QT43" s="8">
+        <v>0.81786596420059243</v>
+      </c>
+      <c r="QU43" s="8">
+        <v>101.6609</v>
+      </c>
+      <c r="QV43" s="10">
+        <v>15239.509383760982</v>
+      </c>
     </row>
-    <row r="44" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>398</v>
       </c>
@@ -62977,8 +63649,23 @@
       <c r="QQ44">
         <v>4.3745780692448645E-2</v>
       </c>
+      <c r="QR44" s="8">
+        <v>16377.960176766268</v>
+      </c>
+      <c r="QS44" s="8">
+        <v>83.144990000000007</v>
+      </c>
+      <c r="QT44" s="8">
+        <v>0.81786596420059243</v>
+      </c>
+      <c r="QU44" s="8">
+        <v>101.6609</v>
+      </c>
+      <c r="QV44" s="10">
+        <v>15239.509383760982</v>
+      </c>
     </row>
-    <row r="45" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>399</v>
       </c>
@@ -64377,8 +65064,23 @@
       <c r="QQ45">
         <v>3.9249327947258938E-2</v>
       </c>
+      <c r="QR45" s="8">
+        <v>14481.281054492565</v>
+      </c>
+      <c r="QS45" s="8">
+        <v>71.066800000000001</v>
+      </c>
+      <c r="QT45" s="8">
+        <v>0.77748855403701245</v>
+      </c>
+      <c r="QU45" s="8">
+        <v>91.405589999999989</v>
+      </c>
+      <c r="QV45" s="10">
+        <v>14149.193563663512</v>
+      </c>
     </row>
-    <row r="46" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>400</v>
       </c>
@@ -65777,8 +66479,23 @@
       <c r="QQ46">
         <v>3.9249327947258938E-2</v>
       </c>
+      <c r="QR46" s="8">
+        <v>14481.281054492565</v>
+      </c>
+      <c r="QS46" s="8">
+        <v>71.066800000000001</v>
+      </c>
+      <c r="QT46" s="8">
+        <v>0.77748855403701245</v>
+      </c>
+      <c r="QU46" s="8">
+        <v>91.405589999999989</v>
+      </c>
+      <c r="QV46" s="10">
+        <v>14149.193563663512</v>
+      </c>
     </row>
-    <row r="47" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>401</v>
       </c>
@@ -67177,8 +67894,23 @@
       <c r="QQ47">
         <v>3.9249327947258938E-2</v>
       </c>
+      <c r="QR47" s="8">
+        <v>14481.281054492565</v>
+      </c>
+      <c r="QS47" s="8">
+        <v>71.066800000000001</v>
+      </c>
+      <c r="QT47" s="8">
+        <v>0.77748855403701245</v>
+      </c>
+      <c r="QU47" s="8">
+        <v>91.405589999999989</v>
+      </c>
+      <c r="QV47" s="10">
+        <v>14149.193563663512</v>
+      </c>
     </row>
-    <row r="48" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -68577,8 +69309,23 @@
       <c r="QQ48">
         <v>3.9249327947258938E-2</v>
       </c>
+      <c r="QR48" s="8">
+        <v>14481.281054492565</v>
+      </c>
+      <c r="QS48" s="8">
+        <v>71.066800000000001</v>
+      </c>
+      <c r="QT48" s="8">
+        <v>0.77748855403701245</v>
+      </c>
+      <c r="QU48" s="8">
+        <v>91.405589999999989</v>
+      </c>
+      <c r="QV48" s="10">
+        <v>14149.193563663512</v>
+      </c>
     </row>
-    <row r="49" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>403</v>
       </c>
@@ -69977,8 +70724,23 @@
       <c r="QQ49">
         <v>3.8748985145627135E-2</v>
       </c>
+      <c r="QR49" s="8">
+        <v>14639.52620180564</v>
+      </c>
+      <c r="QS49" s="8">
+        <v>70.151800000000009</v>
+      </c>
+      <c r="QT49" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU49" s="8">
+        <v>91.229710000000011</v>
+      </c>
+      <c r="QV49" s="10">
+        <v>14639.52620180564</v>
+      </c>
     </row>
-    <row r="50" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>404</v>
       </c>
@@ -71377,8 +72139,23 @@
       <c r="QQ50">
         <v>3.8748985145627135E-2</v>
       </c>
+      <c r="QR50" s="8">
+        <v>14639.52620180564</v>
+      </c>
+      <c r="QS50" s="8">
+        <v>70.151800000000009</v>
+      </c>
+      <c r="QT50" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU50" s="8">
+        <v>91.229710000000011</v>
+      </c>
+      <c r="QV50" s="10">
+        <v>14639.52620180564</v>
+      </c>
     </row>
-    <row r="51" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -72777,8 +73554,23 @@
       <c r="QQ51">
         <v>3.8748985145627135E-2</v>
       </c>
+      <c r="QR51" s="8">
+        <v>14639.52620180564</v>
+      </c>
+      <c r="QS51" s="8">
+        <v>70.151800000000009</v>
+      </c>
+      <c r="QT51" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU51" s="8">
+        <v>91.229710000000011</v>
+      </c>
+      <c r="QV51" s="10">
+        <v>14639.52620180564</v>
+      </c>
     </row>
-    <row r="52" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>406</v>
       </c>
@@ -74177,8 +74969,23 @@
       <c r="QQ52">
         <v>3.8748985145627135E-2</v>
       </c>
+      <c r="QR52" s="8">
+        <v>14639.52620180564</v>
+      </c>
+      <c r="QS52" s="8">
+        <v>70.151800000000009</v>
+      </c>
+      <c r="QT52" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU52" s="8">
+        <v>91.229710000000011</v>
+      </c>
+      <c r="QV52" s="10">
+        <v>14639.52620180564</v>
+      </c>
     </row>
-    <row r="53" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>407</v>
       </c>
@@ -75577,8 +76384,23 @@
       <c r="QQ53">
         <v>3.6652908597029667E-2</v>
       </c>
+      <c r="QR53" s="8">
+        <v>13301.000973307831</v>
+      </c>
+      <c r="QS53" s="8">
+        <v>61.564436515857054</v>
+      </c>
+      <c r="QT53" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU53" s="8">
+        <v>80.062175021240364</v>
+      </c>
+      <c r="QV53" s="10">
+        <v>13301.000973307831</v>
+      </c>
     </row>
-    <row r="54" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -76978,8 +77800,23 @@
       <c r="QQ54">
         <v>3.6652908597029667E-2</v>
       </c>
+      <c r="QR54" s="8">
+        <v>13301.000973307831</v>
+      </c>
+      <c r="QS54" s="8">
+        <v>61.564436515857054</v>
+      </c>
+      <c r="QT54" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU54" s="8">
+        <v>80.062175021240364</v>
+      </c>
+      <c r="QV54" s="10">
+        <v>13301.000973307831</v>
+      </c>
     </row>
-    <row r="55" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -78379,8 +79216,23 @@
       <c r="QQ55">
         <v>3.6652908597029667E-2</v>
       </c>
+      <c r="QR55" s="8">
+        <v>13301.000973307831</v>
+      </c>
+      <c r="QS55" s="8">
+        <v>61.564436515857054</v>
+      </c>
+      <c r="QT55" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU55" s="8">
+        <v>80.062175021240364</v>
+      </c>
+      <c r="QV55" s="10">
+        <v>13301.000973307831</v>
+      </c>
     </row>
-    <row r="56" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>410</v>
       </c>
@@ -79780,8 +80632,23 @@
       <c r="QQ56">
         <v>3.6652908597029667E-2</v>
       </c>
+      <c r="QR56" s="8">
+        <v>13301.000973307831</v>
+      </c>
+      <c r="QS56" s="8">
+        <v>61.564436515857054</v>
+      </c>
+      <c r="QT56" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU56" s="8">
+        <v>80.062175021240364</v>
+      </c>
+      <c r="QV56" s="10">
+        <v>13301.000973307831</v>
+      </c>
     </row>
-    <row r="57" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>411</v>
       </c>
@@ -81181,8 +82048,23 @@
       <c r="QQ57">
         <v>3.7003696714082698E-2</v>
       </c>
+      <c r="QR57" s="8">
+        <v>13835.722339237102</v>
+      </c>
+      <c r="QS57" s="8">
+        <v>61.855910992365288</v>
+      </c>
+      <c r="QT57" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU57" s="8">
+        <v>80.441226335165993</v>
+      </c>
+      <c r="QV57" s="10">
+        <v>13835.722339237102</v>
+      </c>
     </row>
-    <row r="58" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>412</v>
       </c>
@@ -82582,8 +83464,23 @@
       <c r="QQ58">
         <v>3.7003696714082698E-2</v>
       </c>
+      <c r="QR58" s="8">
+        <v>13835.722339237102</v>
+      </c>
+      <c r="QS58" s="8">
+        <v>61.855910992365288</v>
+      </c>
+      <c r="QT58" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU58" s="8">
+        <v>80.441226335165993</v>
+      </c>
+      <c r="QV58" s="10">
+        <v>13835.722339237102</v>
+      </c>
     </row>
-    <row r="59" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>413</v>
       </c>
@@ -83983,8 +84880,23 @@
       <c r="QQ59">
         <v>3.7003696714082698E-2</v>
       </c>
+      <c r="QR59" s="8">
+        <v>13835.722339237102</v>
+      </c>
+      <c r="QS59" s="8">
+        <v>61.855910992365288</v>
+      </c>
+      <c r="QT59" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU59" s="8">
+        <v>80.441226335165993</v>
+      </c>
+      <c r="QV59" s="10">
+        <v>13835.722339237102</v>
+      </c>
     </row>
-    <row r="60" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>414</v>
       </c>
@@ -85384,8 +86296,23 @@
       <c r="QQ60">
         <v>3.7003696714082698E-2</v>
       </c>
+      <c r="QR60" s="8">
+        <v>13835.722339237102</v>
+      </c>
+      <c r="QS60" s="8">
+        <v>61.855910992365288</v>
+      </c>
+      <c r="QT60" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU60" s="8">
+        <v>80.441226335165993</v>
+      </c>
+      <c r="QV60" s="10">
+        <v>13835.722339237102</v>
+      </c>
     </row>
-    <row r="61" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>415</v>
       </c>
@@ -86785,8 +87712,23 @@
       <c r="QQ61">
         <v>4.9064199079882895E-2</v>
       </c>
+      <c r="QR61" s="8">
+        <v>14322.021627963337</v>
+      </c>
+      <c r="QS61" s="8">
+        <v>61.846828720176127</v>
+      </c>
+      <c r="QT61" s="8">
+        <v>0.76895783182912669</v>
+      </c>
+      <c r="QU61" s="8">
+        <v>80.429415190506006</v>
+      </c>
+      <c r="QV61" s="10">
+        <v>14322.021627963337</v>
+      </c>
     </row>
-    <row r="62" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF62" s="1"/>
       <c r="LG62" s="1"/>
       <c r="LH62" s="1"/>
@@ -86832,7 +87774,7 @@
       <c r="QF62" s="5"/>
       <c r="QK62" s="6"/>
     </row>
-    <row r="63" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF63" s="1"/>
       <c r="LG63" s="1"/>
       <c r="LH63" s="1"/>
@@ -86878,7 +87820,7 @@
       <c r="QF63" s="5"/>
       <c r="QK63" s="6"/>
     </row>
-    <row r="64" spans="1:459" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF64" s="1"/>
       <c r="LG64" s="1"/>
       <c r="LH64" s="1"/>
@@ -86938,7 +87880,7 @@
       <c r="QF68" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
opdatering på mange ting
</commit_message>
<xml_diff>
--- a/AAMK.xlsx
+++ b/AAMK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon ik mig\Desktop\9. Semester\Arbejdsmarkeds projekt\Empirisk-SFC-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF15935-6F3C-429F-861F-3F1A1F892DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F08EBF-263B-49EF-A02F-6AC84414F01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="526">
   <si>
     <t>IBA_h</t>
   </si>
@@ -1605,15 +1605,28 @@
   <si>
     <t>tydd</t>
   </si>
+  <si>
+    <t>obs_dp_q_test</t>
+  </si>
+  <si>
+    <t>wage_dp_q_test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1681,23 +1694,26 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2014,11 +2030,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:QV68"/>
+  <dimension ref="A1:QX68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="QK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="QW2" sqref="QW2"/>
+      <selection pane="topRight" activeCell="QV6" sqref="QV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,7 +2042,7 @@
     <col min="456" max="456" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>496</v>
       </c>
@@ -3419,8 +3435,14 @@
       <c r="QV1" s="10" t="s">
         <v>523</v>
       </c>
+      <c r="QW1" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="QX1" s="11" t="s">
+        <v>525</v>
+      </c>
     </row>
-    <row r="2" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -4814,8 +4836,14 @@
       <c r="QV2" s="10">
         <v>19029</v>
       </c>
+      <c r="QW2">
+        <v>42.511000000000003</v>
+      </c>
+      <c r="QX2">
+        <v>42.511000000000003</v>
+      </c>
     </row>
-    <row r="3" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>357</v>
       </c>
@@ -6209,8 +6237,14 @@
       <c r="QV3" s="10">
         <v>19029</v>
       </c>
+      <c r="QW3">
+        <v>42.511000000000003</v>
+      </c>
+      <c r="QX3">
+        <v>42.511000000000003</v>
+      </c>
     </row>
-    <row r="4" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -7604,8 +7638,14 @@
       <c r="QV4" s="10">
         <v>19029</v>
       </c>
+      <c r="QW4">
+        <v>42.511000000000003</v>
+      </c>
+      <c r="QX4">
+        <v>42.511000000000003</v>
+      </c>
     </row>
-    <row r="5" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -8999,8 +9039,14 @@
       <c r="QV5" s="10">
         <v>14617</v>
       </c>
+      <c r="QW5">
+        <v>43.361220000000003</v>
+      </c>
+      <c r="QX5">
+        <v>44.168928999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -10394,8 +10440,14 @@
       <c r="QV6" s="10">
         <v>14617</v>
       </c>
+      <c r="QW6">
+        <v>43.361220000000003</v>
+      </c>
+      <c r="QX6">
+        <v>44.168928999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -11789,8 +11841,14 @@
       <c r="QV7" s="10">
         <v>14617</v>
       </c>
+      <c r="QW7">
+        <v>43.361220000000003</v>
+      </c>
+      <c r="QX7">
+        <v>44.168928999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -13184,8 +13242,14 @@
       <c r="QV8" s="10">
         <v>14617</v>
       </c>
+      <c r="QW8">
+        <v>43.361220000000003</v>
+      </c>
+      <c r="QX8">
+        <v>44.168928999999999</v>
+      </c>
     </row>
-    <row r="9" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>363</v>
       </c>
@@ -14579,8 +14643,14 @@
       <c r="QV9" s="10">
         <v>10407</v>
       </c>
+      <c r="QW9">
+        <v>44.228444400000001</v>
+      </c>
+      <c r="QX9">
+        <v>46.068362990999987</v>
+      </c>
     </row>
-    <row r="10" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -15974,8 +16044,14 @@
       <c r="QV10" s="10">
         <v>10407</v>
       </c>
+      <c r="QW10">
+        <v>44.228444400000001</v>
+      </c>
+      <c r="QX10">
+        <v>46.068362990999987</v>
+      </c>
     </row>
-    <row r="11" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>365</v>
       </c>
@@ -17369,8 +17445,14 @@
       <c r="QV11" s="10">
         <v>10407</v>
       </c>
+      <c r="QW11">
+        <v>44.228444400000001</v>
+      </c>
+      <c r="QX11">
+        <v>46.068362990999987</v>
+      </c>
     </row>
-    <row r="12" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -18764,8 +18846,14 @@
       <c r="QV12" s="10">
         <v>10407</v>
       </c>
+      <c r="QW12">
+        <v>44.228444400000001</v>
+      </c>
+      <c r="QX12">
+        <v>46.068362990999987</v>
+      </c>
     </row>
-    <row r="13" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>367</v>
       </c>
@@ -20159,8 +20247,14 @@
       <c r="QV13" s="10">
         <v>6955</v>
       </c>
+      <c r="QW13">
+        <v>45.113013288000012</v>
+      </c>
+      <c r="QX13">
+        <v>48.234107439076993</v>
+      </c>
     </row>
-    <row r="14" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -21554,8 +21648,14 @@
       <c r="QV14" s="10">
         <v>6955</v>
       </c>
+      <c r="QW14">
+        <v>45.113013288000012</v>
+      </c>
+      <c r="QX14">
+        <v>48.234107439076993</v>
+      </c>
     </row>
-    <row r="15" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>369</v>
       </c>
@@ -22949,8 +23049,14 @@
       <c r="QV15" s="10">
         <v>6955</v>
       </c>
+      <c r="QW15">
+        <v>45.113013288000012</v>
+      </c>
+      <c r="QX15">
+        <v>48.234107439076993</v>
+      </c>
     </row>
-    <row r="16" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>370</v>
       </c>
@@ -24344,8 +24450,14 @@
       <c r="QV16" s="10">
         <v>6955</v>
       </c>
+      <c r="QW16">
+        <v>45.113013288000012</v>
+      </c>
+      <c r="QX16">
+        <v>48.234107439076993</v>
+      </c>
     </row>
-    <row r="17" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>371</v>
       </c>
@@ -25739,8 +25851,14 @@
       <c r="QV17" s="10">
         <v>14571</v>
       </c>
+      <c r="QW17">
+        <v>46.015273553759997</v>
+      </c>
+      <c r="QX17">
+        <v>49.731857244160011</v>
+      </c>
     </row>
-    <row r="18" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -27134,8 +27252,14 @@
       <c r="QV18" s="10">
         <v>14571</v>
       </c>
+      <c r="QW18">
+        <v>46.015273553759997</v>
+      </c>
+      <c r="QX18">
+        <v>49.731857244160011</v>
+      </c>
     </row>
-    <row r="19" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>373</v>
       </c>
@@ -28529,8 +28653,14 @@
       <c r="QV19" s="10">
         <v>14571</v>
       </c>
+      <c r="QW19">
+        <v>46.015273553759997</v>
+      </c>
+      <c r="QX19">
+        <v>49.731857244160011</v>
+      </c>
     </row>
-    <row r="20" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>374</v>
       </c>
@@ -29924,8 +30054,14 @@
       <c r="QV20" s="10">
         <v>14571</v>
       </c>
+      <c r="QW20">
+        <v>46.015273553759997</v>
+      </c>
+      <c r="QX20">
+        <v>49.731857244160011</v>
+      </c>
     </row>
-    <row r="21" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>375</v>
       </c>
@@ -31319,8 +31455,14 @@
       <c r="QV21" s="10">
         <v>18082.780340742898</v>
       </c>
+      <c r="QW21">
+        <v>46.935579024835199</v>
+      </c>
+      <c r="QX21">
+        <v>51.472949979062662</v>
+      </c>
     </row>
-    <row r="22" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -32714,8 +32856,14 @@
       <c r="QV22" s="10">
         <v>18082.780340742898</v>
       </c>
+      <c r="QW22">
+        <v>46.935579024835199</v>
+      </c>
+      <c r="QX22">
+        <v>51.472949979062662</v>
+      </c>
     </row>
-    <row r="23" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>377</v>
       </c>
@@ -34109,8 +34257,14 @@
       <c r="QV23" s="10">
         <v>18082.780340742898</v>
       </c>
+      <c r="QW23">
+        <v>46.935579024835199</v>
+      </c>
+      <c r="QX23">
+        <v>51.472949979062662</v>
+      </c>
     </row>
-    <row r="24" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -35504,8 +35658,14 @@
       <c r="QV24" s="10">
         <v>18082.780340742898</v>
       </c>
+      <c r="QW24">
+        <v>46.935579024835199</v>
+      </c>
+      <c r="QX24">
+        <v>51.472949979062662</v>
+      </c>
     </row>
-    <row r="25" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -36899,8 +37059,14 @@
       <c r="QV25" s="10">
         <v>17011.423221768997</v>
       </c>
+      <c r="QW25">
+        <v>47.874290605331907</v>
+      </c>
+      <c r="QX25">
+        <v>52.560544252059493</v>
+      </c>
     </row>
-    <row r="26" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -38294,8 +38460,14 @@
       <c r="QV26" s="10">
         <v>17011.423221768997</v>
       </c>
+      <c r="QW26">
+        <v>47.874290605331907</v>
+      </c>
+      <c r="QX26">
+        <v>52.560544252059493</v>
+      </c>
     </row>
-    <row r="27" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>381</v>
       </c>
@@ -39689,8 +39861,14 @@
       <c r="QV27" s="10">
         <v>17011.423221768997</v>
       </c>
+      <c r="QW27">
+        <v>47.874290605331907</v>
+      </c>
+      <c r="QX27">
+        <v>52.560544252059493</v>
+      </c>
     </row>
-    <row r="28" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>382</v>
       </c>
@@ -41084,8 +41262,14 @@
       <c r="QV28" s="10">
         <v>17011.423221768997</v>
       </c>
+      <c r="QW28">
+        <v>47.874290605331907</v>
+      </c>
+      <c r="QX28">
+        <v>52.560544252059493</v>
+      </c>
     </row>
-    <row r="29" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -42479,8 +42663,14 @@
       <c r="QV29" s="10">
         <v>18883.449153889494</v>
       </c>
+      <c r="QW29">
+        <v>48.831776417438547</v>
+      </c>
+      <c r="QX29">
+        <v>53.721124205871959</v>
+      </c>
     </row>
-    <row r="30" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>384</v>
       </c>
@@ -43874,8 +44064,14 @@
       <c r="QV30" s="10">
         <v>18883.449153889494</v>
       </c>
+      <c r="QW30">
+        <v>48.831776417438547</v>
+      </c>
+      <c r="QX30">
+        <v>53.721124205871959</v>
+      </c>
     </row>
-    <row r="31" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>385</v>
       </c>
@@ -45269,8 +45465,14 @@
       <c r="QV31" s="10">
         <v>18883.449153889494</v>
       </c>
+      <c r="QW31">
+        <v>48.831776417438547</v>
+      </c>
+      <c r="QX31">
+        <v>53.721124205871959</v>
+      </c>
     </row>
-    <row r="32" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>386</v>
       </c>
@@ -46684,8 +46886,14 @@
       <c r="QV32" s="10">
         <v>18883.449153889494</v>
       </c>
+      <c r="QW32">
+        <v>48.831776417438547</v>
+      </c>
+      <c r="QX32">
+        <v>53.721124205871959</v>
+      </c>
     </row>
-    <row r="33" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -48099,8 +48307,14 @@
       <c r="QV33" s="10">
         <v>17305.191954202463</v>
       </c>
+      <c r="QW33">
+        <v>49.80841194578732</v>
+      </c>
+      <c r="QX33">
+        <v>54.693900908124789</v>
+      </c>
     </row>
-    <row r="34" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -49514,8 +49728,14 @@
       <c r="QV34" s="10">
         <v>17305.191954202463</v>
       </c>
+      <c r="QW34">
+        <v>49.80841194578732</v>
+      </c>
+      <c r="QX34">
+        <v>54.693900908124789</v>
+      </c>
     </row>
-    <row r="35" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>389</v>
       </c>
@@ -50929,8 +51149,14 @@
       <c r="QV35" s="10">
         <v>17305.191954202463</v>
       </c>
+      <c r="QW35">
+        <v>49.80841194578732</v>
+      </c>
+      <c r="QX35">
+        <v>54.693900908124789</v>
+      </c>
     </row>
-    <row r="36" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -52344,8 +52570,14 @@
       <c r="QV36" s="10">
         <v>17305.191954202463</v>
       </c>
+      <c r="QW36">
+        <v>49.80841194578732</v>
+      </c>
+      <c r="QX36">
+        <v>54.693900908124789</v>
+      </c>
     </row>
-    <row r="37" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>391</v>
       </c>
@@ -53759,8 +53991,14 @@
       <c r="QV37" s="10">
         <v>15672.358399246803</v>
       </c>
+      <c r="QW37">
+        <v>50.80458018470307</v>
+      </c>
+      <c r="QX37">
+        <v>56.938263092197772</v>
+      </c>
     </row>
-    <row r="38" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>392</v>
       </c>
@@ -55174,8 +55412,14 @@
       <c r="QV38" s="10">
         <v>15672.358399246803</v>
       </c>
+      <c r="QW38">
+        <v>50.80458018470307</v>
+      </c>
+      <c r="QX38">
+        <v>56.938263092197772</v>
+      </c>
     </row>
-    <row r="39" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>393</v>
       </c>
@@ -56589,8 +56833,14 @@
       <c r="QV39" s="10">
         <v>15672.358399246803</v>
       </c>
+      <c r="QW39">
+        <v>50.80458018470307</v>
+      </c>
+      <c r="QX39">
+        <v>56.938263092197772</v>
+      </c>
     </row>
-    <row r="40" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>394</v>
       </c>
@@ -58004,8 +58254,14 @@
       <c r="QV40" s="10">
         <v>15672.358399246803</v>
       </c>
+      <c r="QW40">
+        <v>50.80458018470307</v>
+      </c>
+      <c r="QX40">
+        <v>56.938263092197772</v>
+      </c>
     </row>
-    <row r="41" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -59419,8 +59675,14 @@
       <c r="QV41" s="10">
         <v>15239.509383760982</v>
       </c>
+      <c r="QW41">
+        <v>51.820671788397128</v>
+      </c>
+      <c r="QX41">
+        <v>56.578974135619227</v>
+      </c>
     </row>
-    <row r="42" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>396</v>
       </c>
@@ -60834,8 +61096,14 @@
       <c r="QV42" s="10">
         <v>15239.509383760982</v>
       </c>
+      <c r="QW42">
+        <v>51.820671788397128</v>
+      </c>
+      <c r="QX42">
+        <v>56.578974135619227</v>
+      </c>
     </row>
-    <row r="43" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>397</v>
       </c>
@@ -62249,8 +62517,14 @@
       <c r="QV43" s="10">
         <v>15239.509383760982</v>
       </c>
+      <c r="QW43">
+        <v>51.820671788397128</v>
+      </c>
+      <c r="QX43">
+        <v>56.578974135619227</v>
+      </c>
     </row>
-    <row r="44" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>398</v>
       </c>
@@ -63664,8 +63938,14 @@
       <c r="QV44" s="10">
         <v>15239.509383760982</v>
       </c>
+      <c r="QW44">
+        <v>51.820671788397128</v>
+      </c>
+      <c r="QX44">
+        <v>56.578974135619227</v>
+      </c>
     </row>
-    <row r="45" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>399</v>
       </c>
@@ -65079,8 +65359,14 @@
       <c r="QV45" s="10">
         <v>14149.193563663512</v>
       </c>
+      <c r="QW45">
+        <v>52.390699178069497</v>
+      </c>
+      <c r="QX45">
+        <v>56.987053267724441</v>
+      </c>
     </row>
-    <row r="46" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>400</v>
       </c>
@@ -66494,8 +66780,14 @@
       <c r="QV46" s="10">
         <v>14149.193563663512</v>
       </c>
+      <c r="QW46">
+        <v>52.390699178069497</v>
+      </c>
+      <c r="QX46">
+        <v>56.987053267724441</v>
+      </c>
     </row>
-    <row r="47" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>401</v>
       </c>
@@ -67909,8 +68201,14 @@
       <c r="QV47" s="10">
         <v>14149.193563663512</v>
       </c>
+      <c r="QW47">
+        <v>52.390699178069497</v>
+      </c>
+      <c r="QX47">
+        <v>56.987053267724441</v>
+      </c>
     </row>
-    <row r="48" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -69324,8 +69622,14 @@
       <c r="QV48" s="10">
         <v>14149.193563663512</v>
       </c>
+      <c r="QW48">
+        <v>52.390699178069497</v>
+      </c>
+      <c r="QX48">
+        <v>56.987053267724441</v>
+      </c>
     </row>
-    <row r="49" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>403</v>
       </c>
@@ -70739,8 +71043,14 @@
       <c r="QV49" s="10">
         <v>14639.52620180564</v>
       </c>
+      <c r="QW49">
+        <v>53.22895036491861</v>
+      </c>
+      <c r="QX49">
+        <v>59.213222522235071</v>
+      </c>
     </row>
-    <row r="50" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>404</v>
       </c>
@@ -72154,8 +72464,14 @@
       <c r="QV50" s="10">
         <v>14639.52620180564</v>
       </c>
+      <c r="QW50">
+        <v>53.22895036491861</v>
+      </c>
+      <c r="QX50">
+        <v>59.213222522235071</v>
+      </c>
     </row>
-    <row r="51" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -73569,8 +73885,14 @@
       <c r="QV51" s="10">
         <v>14639.52620180564</v>
       </c>
+      <c r="QW51">
+        <v>53.22895036491861</v>
+      </c>
+      <c r="QX51">
+        <v>59.213222522235071</v>
+      </c>
     </row>
-    <row r="52" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>406</v>
       </c>
@@ -74984,8 +75306,14 @@
       <c r="QV52" s="10">
         <v>14639.52620180564</v>
       </c>
+      <c r="QW52">
+        <v>53.22895036491861</v>
+      </c>
+      <c r="QX52">
+        <v>59.213222522235071</v>
+      </c>
     </row>
-    <row r="53" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>407</v>
       </c>
@@ -76399,8 +76727,14 @@
       <c r="QV53" s="10">
         <v>13301.000973307831</v>
       </c>
+      <c r="QW53">
+        <v>53.894312244480091</v>
+      </c>
+      <c r="QX53">
+        <v>60.105897706013721</v>
+      </c>
     </row>
-    <row r="54" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -77815,8 +78149,14 @@
       <c r="QV54" s="10">
         <v>13301.000973307831</v>
       </c>
+      <c r="QW54">
+        <v>53.894312244480091</v>
+      </c>
+      <c r="QX54">
+        <v>60.105897706013721</v>
+      </c>
     </row>
-    <row r="55" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -79231,8 +79571,14 @@
       <c r="QV55" s="10">
         <v>13301.000973307831</v>
       </c>
+      <c r="QW55">
+        <v>53.894312244480091</v>
+      </c>
+      <c r="QX55">
+        <v>60.105897706013721</v>
+      </c>
     </row>
-    <row r="56" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>410</v>
       </c>
@@ -80647,8 +80993,14 @@
       <c r="QV56" s="10">
         <v>13301.000973307831</v>
       </c>
+      <c r="QW56">
+        <v>53.894312244480091</v>
+      </c>
+      <c r="QX56">
+        <v>60.105897706013721</v>
+      </c>
     </row>
-    <row r="57" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>411</v>
       </c>
@@ -82063,8 +82415,14 @@
       <c r="QV57" s="10">
         <v>13835.722339237102</v>
       </c>
+      <c r="QW57">
+        <v>54.567991147536091</v>
+      </c>
+      <c r="QX57">
+        <v>61.728756944076082</v>
+      </c>
     </row>
-    <row r="58" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>412</v>
       </c>
@@ -83479,8 +83837,14 @@
       <c r="QV58" s="10">
         <v>13835.722339237102</v>
       </c>
+      <c r="QW58">
+        <v>54.567991147536091</v>
+      </c>
+      <c r="QX58">
+        <v>61.728756944076082</v>
+      </c>
     </row>
-    <row r="59" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>413</v>
       </c>
@@ -84895,8 +85259,14 @@
       <c r="QV59" s="10">
         <v>13835.722339237102</v>
       </c>
+      <c r="QW59">
+        <v>54.567991147536091</v>
+      </c>
+      <c r="QX59">
+        <v>61.728756944076082</v>
+      </c>
     </row>
-    <row r="60" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>414</v>
       </c>
@@ -86311,8 +86681,14 @@
       <c r="QV60" s="10">
         <v>13835.722339237102</v>
       </c>
+      <c r="QW60">
+        <v>54.567991147536091</v>
+      </c>
+      <c r="QX60">
+        <v>61.728756944076082</v>
+      </c>
     </row>
-    <row r="61" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>415</v>
       </c>
@@ -87727,8 +88103,14 @@
       <c r="QV61" s="10">
         <v>14322.021627963337</v>
       </c>
+      <c r="QW61">
+        <v>55.195523045732763</v>
+      </c>
+      <c r="QX61">
+        <v>64.327702562135926</v>
+      </c>
     </row>
-    <row r="62" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF62" s="1"/>
       <c r="LG62" s="1"/>
       <c r="LH62" s="1"/>
@@ -87774,7 +88156,7 @@
       <c r="QF62" s="5"/>
       <c r="QK62" s="6"/>
     </row>
-    <row r="63" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF63" s="1"/>
       <c r="LG63" s="1"/>
       <c r="LH63" s="1"/>
@@ -87820,7 +88202,7 @@
       <c r="QF63" s="5"/>
       <c r="QK63" s="6"/>
     </row>
-    <row r="64" spans="1:464" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF64" s="1"/>
       <c r="LG64" s="1"/>
       <c r="LH64" s="1"/>
@@ -87880,7 +88262,7 @@
       <c r="QF68" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ser ud til der er et langsigtet forhold
</commit_message>
<xml_diff>
--- a/AAMK.xlsx
+++ b/AAMK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon ik mig\Desktop\9. Semester\Arbejdsmarkeds projekt\Empirisk-SFC-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjkss\Desktop\9. semester\Empirisk-SFC-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F08EBF-263B-49EF-A02F-6AC84414F01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3147771-D839-4970-BE12-600EBB9A199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="527">
   <si>
     <t>IBA_h</t>
   </si>
@@ -1611,6 +1611,9 @@
   <si>
     <t>wage_dp_q_test</t>
   </si>
+  <si>
+    <t>SD4</t>
+  </si>
 </sst>
 </file>
 
@@ -2030,11 +2033,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:QX68"/>
+  <dimension ref="A1:QZ68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="QK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="QV6" sqref="QV6"/>
+      <pane xSplit="1" topLeftCell="QM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="QY3" sqref="QY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,7 +2045,7 @@
     <col min="456" max="456" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>496</v>
       </c>
@@ -3441,8 +3444,14 @@
       <c r="QX1" s="11" t="s">
         <v>525</v>
       </c>
+      <c r="QY1" t="s">
+        <v>526</v>
+      </c>
+      <c r="QZ1" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="2" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -4842,8 +4851,14 @@
       <c r="QX2">
         <v>42.511000000000003</v>
       </c>
+      <c r="QY2">
+        <v>0</v>
+      </c>
+      <c r="QZ2">
+        <v>89.95736181431883</v>
+      </c>
     </row>
-    <row r="3" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>357</v>
       </c>
@@ -6243,8 +6258,14 @@
       <c r="QX3">
         <v>42.511000000000003</v>
       </c>
+      <c r="QY3">
+        <v>0</v>
+      </c>
+      <c r="QZ3">
+        <v>90.135565815589473</v>
+      </c>
     </row>
-    <row r="4" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -7644,8 +7665,14 @@
       <c r="QX4">
         <v>42.511000000000003</v>
       </c>
+      <c r="QY4">
+        <v>1</v>
+      </c>
+      <c r="QZ4">
+        <v>90.385051331830496</v>
+      </c>
     </row>
-    <row r="5" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -9045,8 +9072,14 @@
       <c r="QX5">
         <v>44.168928999999999</v>
       </c>
+      <c r="QY5">
+        <v>0</v>
+      </c>
+      <c r="QZ5">
+        <v>90.705818469964285</v>
+      </c>
     </row>
-    <row r="6" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -10446,8 +10479,14 @@
       <c r="QX6">
         <v>44.168928999999999</v>
       </c>
+      <c r="QY6">
+        <v>0</v>
+      </c>
+      <c r="QZ6">
+        <v>91.775042263743515</v>
+      </c>
     </row>
-    <row r="7" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -11847,8 +11886,14 @@
       <c r="QX7">
         <v>44.168928999999999</v>
       </c>
+      <c r="QY7">
+        <v>0</v>
+      </c>
+      <c r="QZ7">
+        <v>91.846323885636252</v>
+      </c>
     </row>
-    <row r="8" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -13248,8 +13293,14 @@
       <c r="QX8">
         <v>44.168928999999999</v>
       </c>
+      <c r="QY8">
+        <v>1</v>
+      </c>
+      <c r="QZ8">
+        <v>91.917605507529004</v>
+      </c>
     </row>
-    <row r="9" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>363</v>
       </c>
@@ -14649,8 +14700,14 @@
       <c r="QX9">
         <v>46.068362990999987</v>
       </c>
+      <c r="QY9">
+        <v>0</v>
+      </c>
+      <c r="QZ9">
+        <v>92.41657654001105</v>
+      </c>
     </row>
-    <row r="10" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -16050,8 +16107,14 @@
       <c r="QX10">
         <v>46.068362990999987</v>
       </c>
+      <c r="QY10">
+        <v>0</v>
+      </c>
+      <c r="QZ10">
+        <v>93.236314817549257</v>
+      </c>
     </row>
-    <row r="11" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>365</v>
       </c>
@@ -17451,8 +17514,14 @@
       <c r="QX11">
         <v>46.068362990999987</v>
       </c>
+      <c r="QY11">
+        <v>0</v>
+      </c>
+      <c r="QZ11">
+        <v>92.879906921930285</v>
+      </c>
     </row>
-    <row r="12" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -18852,8 +18921,14 @@
       <c r="QX12">
         <v>46.068362990999987</v>
       </c>
+      <c r="QY12">
+        <v>1</v>
+      </c>
+      <c r="QZ12">
+        <v>93.913489851301989</v>
+      </c>
     </row>
-    <row r="13" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>367</v>
       </c>
@@ -20253,8 +20328,14 @@
       <c r="QX13">
         <v>48.234107439076993</v>
       </c>
+      <c r="QY13">
+        <v>0</v>
+      </c>
+      <c r="QZ13">
+        <v>95.232199268244628</v>
+      </c>
     </row>
-    <row r="14" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -21654,8 +21735,14 @@
       <c r="QX14">
         <v>48.234107439076993</v>
       </c>
+      <c r="QY14">
+        <v>0</v>
+      </c>
+      <c r="QZ14">
+        <v>96.515267820779712</v>
+      </c>
     </row>
-    <row r="15" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>369</v>
       </c>
@@ -23055,8 +23142,14 @@
       <c r="QX15">
         <v>48.234107439076993</v>
       </c>
+      <c r="QY15">
+        <v>0</v>
+      </c>
+      <c r="QZ15">
+        <v>96.764753337020736</v>
+      </c>
     </row>
-    <row r="16" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>370</v>
       </c>
@@ -24456,8 +24549,14 @@
       <c r="QX16">
         <v>48.234107439076993</v>
       </c>
+      <c r="QY16">
+        <v>1</v>
+      </c>
+      <c r="QZ16">
+        <v>96.657830957642801</v>
+      </c>
     </row>
-    <row r="17" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>371</v>
       </c>
@@ -25857,8 +25956,14 @@
       <c r="QX17">
         <v>49.731857244160011</v>
       </c>
+      <c r="QY17">
+        <v>0</v>
+      </c>
+      <c r="QZ17">
+        <v>96.907316473883853</v>
+      </c>
     </row>
-    <row r="18" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -27258,8 +27363,14 @@
       <c r="QX18">
         <v>49.731857244160011</v>
       </c>
+      <c r="QY18">
+        <v>0</v>
+      </c>
+      <c r="QZ18">
+        <v>97.691413993936848</v>
+      </c>
     </row>
-    <row r="19" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>373</v>
       </c>
@@ -28659,8 +28770,14 @@
       <c r="QX19">
         <v>49.731857244160011</v>
       </c>
+      <c r="QY19">
+        <v>0</v>
+      </c>
+      <c r="QZ19">
+        <v>97.727054751422045</v>
+      </c>
     </row>
-    <row r="20" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>374</v>
       </c>
@@ -30060,8 +30177,14 @@
       <c r="QX20">
         <v>49.731857244160011</v>
       </c>
+      <c r="QY20">
+        <v>1</v>
+      </c>
+      <c r="QZ20">
+        <v>97.869617888285134</v>
+      </c>
     </row>
-    <row r="21" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>375</v>
       </c>
@@ -31461,8 +31584,14 @@
       <c r="QX21">
         <v>51.472949979062662</v>
       </c>
+      <c r="QY21">
+        <v>0</v>
+      </c>
+      <c r="QZ21">
+        <v>98.938841682064378</v>
+      </c>
     </row>
-    <row r="22" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -32862,8 +32991,14 @@
       <c r="QX22">
         <v>51.472949979062662</v>
       </c>
+      <c r="QY22">
+        <v>0</v>
+      </c>
+      <c r="QZ22">
+        <v>99.829861581495308</v>
+      </c>
     </row>
-    <row r="23" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>377</v>
       </c>
@@ -34263,8 +34398,14 @@
       <c r="QX23">
         <v>51.472949979062662</v>
       </c>
+      <c r="QY23">
+        <v>0</v>
+      </c>
+      <c r="QZ23">
+        <v>100.04370634025118</v>
+      </c>
     </row>
-    <row r="24" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -35664,8 +35805,14 @@
       <c r="QX24">
         <v>51.472949979062662</v>
       </c>
+      <c r="QY24">
+        <v>1</v>
+      </c>
+      <c r="QZ24">
+        <v>100.40011423587012</v>
+      </c>
     </row>
-    <row r="25" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -37065,8 +37212,14 @@
       <c r="QX25">
         <v>52.560544252059493</v>
       </c>
+      <c r="QY25">
+        <v>0</v>
+      </c>
+      <c r="QZ25">
+        <v>101.61190116651247</v>
+      </c>
     </row>
-    <row r="26" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -38466,8 +38619,14 @@
       <c r="QX26">
         <v>52.560544252059493</v>
       </c>
+      <c r="QY26">
+        <v>0</v>
+      </c>
+      <c r="QZ26">
+        <v>102.85932896156237</v>
+      </c>
     </row>
-    <row r="27" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>381</v>
       </c>
@@ -39867,8 +40026,14 @@
       <c r="QX27">
         <v>52.560544252059493</v>
       </c>
+      <c r="QY27">
+        <v>0</v>
+      </c>
+      <c r="QZ27">
+        <v>102.75240658218445</v>
+      </c>
     </row>
-    <row r="28" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>382</v>
       </c>
@@ -41268,8 +41433,14 @@
       <c r="QX28">
         <v>52.560544252059493</v>
       </c>
+      <c r="QY28">
+        <v>1</v>
+      </c>
+      <c r="QZ28">
+        <v>103.00189209842549</v>
+      </c>
     </row>
-    <row r="29" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -42669,8 +42840,14 @@
       <c r="QX29">
         <v>53.721124205871959</v>
       </c>
+      <c r="QY29">
+        <v>0</v>
+      </c>
+      <c r="QZ29">
+        <v>104.35624227285329</v>
+      </c>
     </row>
-    <row r="30" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>384</v>
       </c>
@@ -44070,8 +44247,14 @@
       <c r="QX30">
         <v>53.721124205871959</v>
       </c>
+      <c r="QY30">
+        <v>0</v>
+      </c>
+      <c r="QZ30">
+        <v>105.10469892849876</v>
+      </c>
     </row>
-    <row r="31" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>385</v>
       </c>
@@ -45471,8 +45654,14 @@
       <c r="QX31">
         <v>53.721124205871959</v>
       </c>
+      <c r="QY31">
+        <v>0</v>
+      </c>
+      <c r="QZ31">
+        <v>105.28290292976943</v>
+      </c>
     </row>
-    <row r="32" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>386</v>
       </c>
@@ -46892,8 +47081,14 @@
       <c r="QX32">
         <v>53.721124205871959</v>
       </c>
+      <c r="QY32">
+        <v>1</v>
+      </c>
+      <c r="QZ32">
+        <v>105.3185436872546</v>
+      </c>
     </row>
-    <row r="33" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -48313,8 +48508,14 @@
       <c r="QX33">
         <v>54.693900908124789</v>
       </c>
+      <c r="QY33">
+        <v>0</v>
+      </c>
+      <c r="QZ33">
+        <v>105.56802920349563</v>
+      </c>
     </row>
-    <row r="34" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -49734,8 +49935,14 @@
       <c r="QX34">
         <v>54.693900908124789</v>
       </c>
+      <c r="QY34">
+        <v>0</v>
+      </c>
+      <c r="QZ34">
+        <v>105.99571872100734</v>
+      </c>
     </row>
-    <row r="35" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>389</v>
       </c>
@@ -51155,8 +51362,14 @@
       <c r="QX35">
         <v>54.693900908124789</v>
       </c>
+      <c r="QY35">
+        <v>0</v>
+      </c>
+      <c r="QZ35">
+        <v>105.81751482665905</v>
+      </c>
     </row>
-    <row r="36" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -52576,8 +52789,14 @@
       <c r="QX36">
         <v>54.693900908124789</v>
       </c>
+      <c r="QY36">
+        <v>1</v>
+      </c>
+      <c r="QZ36">
+        <v>105.99571872100734</v>
+      </c>
     </row>
-    <row r="37" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>391</v>
       </c>
@@ -53997,8 +54216,14 @@
       <c r="QX37">
         <v>56.938263092197772</v>
       </c>
+      <c r="QY37">
+        <v>0</v>
+      </c>
+      <c r="QZ37">
+        <v>106.20956347976319</v>
+      </c>
     </row>
-    <row r="38" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>392</v>
       </c>
@@ -55418,8 +55643,14 @@
       <c r="QX38">
         <v>56.938263092197772</v>
       </c>
+      <c r="QY38">
+        <v>0</v>
+      </c>
+      <c r="QZ38">
+        <v>106.63725299727486</v>
+      </c>
     </row>
-    <row r="39" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>393</v>
       </c>
@@ -56839,8 +57070,14 @@
       <c r="QX39">
         <v>56.938263092197772</v>
       </c>
+      <c r="QY39">
+        <v>0</v>
+      </c>
+      <c r="QZ39">
+        <v>106.42340823851902</v>
+      </c>
     </row>
-    <row r="40" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>394</v>
       </c>
@@ -58260,8 +58497,14 @@
       <c r="QX40">
         <v>56.938263092197772</v>
       </c>
+      <c r="QY40">
+        <v>1</v>
+      </c>
+      <c r="QZ40">
+        <v>106.49468986041177</v>
+      </c>
     </row>
-    <row r="41" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -59681,8 +59924,14 @@
       <c r="QX41">
         <v>56.578974135619227</v>
       </c>
+      <c r="QY41">
+        <v>0</v>
+      </c>
+      <c r="QZ41">
+        <v>106.49468986041177</v>
+      </c>
     </row>
-    <row r="42" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>396</v>
       </c>
@@ -61102,8 +61351,14 @@
       <c r="QX42">
         <v>56.578974135619227</v>
       </c>
+      <c r="QY42">
+        <v>0</v>
+      </c>
+      <c r="QZ42">
+        <v>107.27878695277528</v>
+      </c>
     </row>
-    <row r="43" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>397</v>
       </c>
@@ -62523,8 +62778,14 @@
       <c r="QX43">
         <v>56.578974135619227</v>
       </c>
+      <c r="QY43">
+        <v>0</v>
+      </c>
+      <c r="QZ43">
+        <v>107.06494219401941</v>
+      </c>
     </row>
-    <row r="44" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>398</v>
       </c>
@@ -63944,8 +64205,14 @@
       <c r="QX44">
         <v>56.578974135619227</v>
       </c>
+      <c r="QY44">
+        <v>1</v>
+      </c>
+      <c r="QZ44">
+        <v>106.85109775603071</v>
+      </c>
     </row>
-    <row r="45" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>399</v>
       </c>
@@ -65365,8 +65632,14 @@
       <c r="QX45">
         <v>56.987053267724441</v>
       </c>
+      <c r="QY45">
+        <v>0</v>
+      </c>
+      <c r="QZ45">
+        <v>106.81545699854553</v>
+      </c>
     </row>
-    <row r="46" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>400</v>
       </c>
@@ -66786,8 +67059,14 @@
       <c r="QX46">
         <v>56.987053267724441</v>
       </c>
+      <c r="QY46">
+        <v>0</v>
+      </c>
+      <c r="QZ46">
+        <v>107.42135083809502</v>
+      </c>
     </row>
-    <row r="47" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>401</v>
       </c>
@@ -68207,8 +68486,14 @@
       <c r="QX47">
         <v>56.987053267724441</v>
       </c>
+      <c r="QY47">
+        <v>0</v>
+      </c>
+      <c r="QZ47">
+        <v>107.24314651605722</v>
+      </c>
     </row>
-    <row r="48" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -69628,8 +69913,14 @@
       <c r="QX48">
         <v>56.987053267724441</v>
       </c>
+      <c r="QY48">
+        <v>1</v>
+      </c>
+      <c r="QZ48">
+        <v>107.27878695277528</v>
+      </c>
     </row>
-    <row r="49" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>403</v>
       </c>
@@ -71049,8 +71340,14 @@
       <c r="QX49">
         <v>59.213222522235071</v>
       </c>
+      <c r="QY49">
+        <v>0</v>
+      </c>
+      <c r="QZ49">
+        <v>107.84904035560675</v>
+      </c>
     </row>
-    <row r="50" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>404</v>
       </c>
@@ -72470,8 +72767,14 @@
       <c r="QX50">
         <v>59.213222522235071</v>
       </c>
+      <c r="QY50">
+        <v>0</v>
+      </c>
+      <c r="QZ50">
+        <v>108.31237030983647</v>
+      </c>
     </row>
-    <row r="51" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -73891,8 +74194,14 @@
       <c r="QX51">
         <v>59.213222522235071</v>
       </c>
+      <c r="QY51">
+        <v>0</v>
+      </c>
+      <c r="QZ51">
+        <v>108.88262264344412</v>
+      </c>
     </row>
-    <row r="52" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>406</v>
       </c>
@@ -75312,8 +75621,14 @@
       <c r="QX52">
         <v>59.213222522235071</v>
       </c>
+      <c r="QY52">
+        <v>1</v>
+      </c>
+      <c r="QZ52">
+        <v>108.63313744797023</v>
+      </c>
     </row>
-    <row r="53" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>407</v>
       </c>
@@ -76733,8 +77048,14 @@
       <c r="QX53">
         <v>60.105897706013721</v>
       </c>
+      <c r="QY53">
+        <v>0</v>
+      </c>
+      <c r="QZ53">
+        <v>108.49057463187427</v>
+      </c>
     </row>
-    <row r="54" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -78155,8 +78476,14 @@
       <c r="QX54">
         <v>60.105897706013721</v>
       </c>
+      <c r="QY54">
+        <v>0</v>
+      </c>
+      <c r="QZ54">
+        <v>109.3815941036157</v>
+      </c>
     </row>
-    <row r="55" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -79577,8 +79904,14 @@
       <c r="QX55">
         <v>60.105897706013721</v>
       </c>
+      <c r="QY55">
+        <v>0</v>
+      </c>
+      <c r="QZ55">
+        <v>109.84492405784543</v>
+      </c>
     </row>
-    <row r="56" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>410</v>
       </c>
@@ -80999,8 +81332,14 @@
       <c r="QX56">
         <v>60.105897706013721</v>
       </c>
+      <c r="QY56">
+        <v>1</v>
+      </c>
+      <c r="QZ56">
+        <v>109.48851648299362</v>
+      </c>
     </row>
-    <row r="57" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>411</v>
       </c>
@@ -82421,8 +82760,14 @@
       <c r="QX57">
         <v>61.728756944076082</v>
       </c>
+      <c r="QY57">
+        <v>0</v>
+      </c>
+      <c r="QZ57">
+        <v>109.77364318440935</v>
+      </c>
     </row>
-    <row r="58" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>412</v>
       </c>
@@ -83843,8 +84188,14 @@
       <c r="QX58">
         <v>61.728756944076082</v>
       </c>
+      <c r="QY58">
+        <v>0</v>
+      </c>
+      <c r="QZ58">
+        <v>110.20133270192103</v>
+      </c>
     </row>
-    <row r="59" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>413</v>
       </c>
@@ -85265,8 +85616,14 @@
       <c r="QX59">
         <v>61.728756944076082</v>
       </c>
+      <c r="QY59">
+        <v>0</v>
+      </c>
+      <c r="QZ59">
+        <v>110.30825508129897</v>
+      </c>
     </row>
-    <row r="60" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>414</v>
       </c>
@@ -86687,8 +87044,14 @@
       <c r="QX60">
         <v>61.728756944076082</v>
       </c>
+      <c r="QY60">
+        <v>1</v>
+      </c>
+      <c r="QZ60">
+        <v>110.23697313863909</v>
+      </c>
     </row>
-    <row r="61" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>415</v>
       </c>
@@ -88109,8 +88472,14 @@
       <c r="QX61">
         <v>64.327702562135926</v>
       </c>
+      <c r="QY61">
+        <v>0</v>
+      </c>
+      <c r="QZ61">
+        <v>110.45081789739493</v>
+      </c>
     </row>
-    <row r="62" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF62" s="1"/>
       <c r="LG62" s="1"/>
       <c r="LH62" s="1"/>
@@ -88156,7 +88525,7 @@
       <c r="QF62" s="5"/>
       <c r="QK62" s="6"/>
     </row>
-    <row r="63" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF63" s="1"/>
       <c r="LG63" s="1"/>
       <c r="LH63" s="1"/>
@@ -88202,7 +88571,7 @@
       <c r="QF63" s="5"/>
       <c r="QK63" s="6"/>
     </row>
-    <row r="64" spans="1:466" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF64" s="1"/>
       <c r="LG64" s="1"/>
       <c r="LH64" s="1"/>

</xml_diff>

<commit_message>
opdateret med nye ligning til at lave shoccks med
</commit_message>
<xml_diff>
--- a/AAMK.xlsx
+++ b/AAMK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjkss\Desktop\9. semester\Empirisk-SFC-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3147771-D839-4970-BE12-600EBB9A199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A43704-6551-4561-BF49-1D1D496818B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="527">
   <si>
     <t>IBA_h</t>
   </si>
@@ -2033,11 +2033,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:QZ68"/>
+  <dimension ref="A1:QY68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="QM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="QY3" sqref="QY3"/>
+      <pane xSplit="1" topLeftCell="QJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="QZ4" sqref="QZ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
     <col min="456" max="456" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>496</v>
       </c>
@@ -3447,11 +3447,8 @@
       <c r="QY1" t="s">
         <v>526</v>
       </c>
-      <c r="QZ1" t="s">
-        <v>511</v>
-      </c>
     </row>
-    <row r="2" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -4854,11 +4851,8 @@
       <c r="QY2">
         <v>0</v>
       </c>
-      <c r="QZ2">
-        <v>89.95736181431883</v>
-      </c>
     </row>
-    <row r="3" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>357</v>
       </c>
@@ -6261,11 +6255,8 @@
       <c r="QY3">
         <v>0</v>
       </c>
-      <c r="QZ3">
-        <v>90.135565815589473</v>
-      </c>
     </row>
-    <row r="4" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -7668,11 +7659,8 @@
       <c r="QY4">
         <v>1</v>
       </c>
-      <c r="QZ4">
-        <v>90.385051331830496</v>
-      </c>
     </row>
-    <row r="5" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -9075,11 +9063,8 @@
       <c r="QY5">
         <v>0</v>
       </c>
-      <c r="QZ5">
-        <v>90.705818469964285</v>
-      </c>
     </row>
-    <row r="6" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -10482,11 +10467,8 @@
       <c r="QY6">
         <v>0</v>
       </c>
-      <c r="QZ6">
-        <v>91.775042263743515</v>
-      </c>
     </row>
-    <row r="7" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>361</v>
       </c>
@@ -11889,11 +11871,8 @@
       <c r="QY7">
         <v>0</v>
       </c>
-      <c r="QZ7">
-        <v>91.846323885636252</v>
-      </c>
     </row>
-    <row r="8" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -13296,11 +13275,8 @@
       <c r="QY8">
         <v>1</v>
       </c>
-      <c r="QZ8">
-        <v>91.917605507529004</v>
-      </c>
     </row>
-    <row r="9" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>363</v>
       </c>
@@ -14703,11 +14679,8 @@
       <c r="QY9">
         <v>0</v>
       </c>
-      <c r="QZ9">
-        <v>92.41657654001105</v>
-      </c>
     </row>
-    <row r="10" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -16110,11 +16083,8 @@
       <c r="QY10">
         <v>0</v>
       </c>
-      <c r="QZ10">
-        <v>93.236314817549257</v>
-      </c>
     </row>
-    <row r="11" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>365</v>
       </c>
@@ -17517,11 +17487,8 @@
       <c r="QY11">
         <v>0</v>
       </c>
-      <c r="QZ11">
-        <v>92.879906921930285</v>
-      </c>
     </row>
-    <row r="12" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -18924,11 +18891,8 @@
       <c r="QY12">
         <v>1</v>
       </c>
-      <c r="QZ12">
-        <v>93.913489851301989</v>
-      </c>
     </row>
-    <row r="13" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>367</v>
       </c>
@@ -20331,11 +20295,8 @@
       <c r="QY13">
         <v>0</v>
       </c>
-      <c r="QZ13">
-        <v>95.232199268244628</v>
-      </c>
     </row>
-    <row r="14" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -21738,11 +21699,8 @@
       <c r="QY14">
         <v>0</v>
       </c>
-      <c r="QZ14">
-        <v>96.515267820779712</v>
-      </c>
     </row>
-    <row r="15" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>369</v>
       </c>
@@ -23145,11 +23103,8 @@
       <c r="QY15">
         <v>0</v>
       </c>
-      <c r="QZ15">
-        <v>96.764753337020736</v>
-      </c>
     </row>
-    <row r="16" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>370</v>
       </c>
@@ -24552,11 +24507,8 @@
       <c r="QY16">
         <v>1</v>
       </c>
-      <c r="QZ16">
-        <v>96.657830957642801</v>
-      </c>
     </row>
-    <row r="17" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>371</v>
       </c>
@@ -25959,11 +25911,8 @@
       <c r="QY17">
         <v>0</v>
       </c>
-      <c r="QZ17">
-        <v>96.907316473883853</v>
-      </c>
     </row>
-    <row r="18" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -27366,11 +27315,8 @@
       <c r="QY18">
         <v>0</v>
       </c>
-      <c r="QZ18">
-        <v>97.691413993936848</v>
-      </c>
     </row>
-    <row r="19" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>373</v>
       </c>
@@ -28773,11 +28719,8 @@
       <c r="QY19">
         <v>0</v>
       </c>
-      <c r="QZ19">
-        <v>97.727054751422045</v>
-      </c>
     </row>
-    <row r="20" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>374</v>
       </c>
@@ -30180,11 +30123,8 @@
       <c r="QY20">
         <v>1</v>
       </c>
-      <c r="QZ20">
-        <v>97.869617888285134</v>
-      </c>
     </row>
-    <row r="21" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>375</v>
       </c>
@@ -31587,11 +31527,8 @@
       <c r="QY21">
         <v>0</v>
       </c>
-      <c r="QZ21">
-        <v>98.938841682064378</v>
-      </c>
     </row>
-    <row r="22" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>376</v>
       </c>
@@ -32994,11 +32931,8 @@
       <c r="QY22">
         <v>0</v>
       </c>
-      <c r="QZ22">
-        <v>99.829861581495308</v>
-      </c>
     </row>
-    <row r="23" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>377</v>
       </c>
@@ -34401,11 +34335,8 @@
       <c r="QY23">
         <v>0</v>
       </c>
-      <c r="QZ23">
-        <v>100.04370634025118</v>
-      </c>
     </row>
-    <row r="24" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>378</v>
       </c>
@@ -35808,11 +35739,8 @@
       <c r="QY24">
         <v>1</v>
       </c>
-      <c r="QZ24">
-        <v>100.40011423587012</v>
-      </c>
     </row>
-    <row r="25" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>379</v>
       </c>
@@ -37215,11 +37143,8 @@
       <c r="QY25">
         <v>0</v>
       </c>
-      <c r="QZ25">
-        <v>101.61190116651247</v>
-      </c>
     </row>
-    <row r="26" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>380</v>
       </c>
@@ -38622,11 +38547,8 @@
       <c r="QY26">
         <v>0</v>
       </c>
-      <c r="QZ26">
-        <v>102.85932896156237</v>
-      </c>
     </row>
-    <row r="27" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>381</v>
       </c>
@@ -40029,11 +39951,8 @@
       <c r="QY27">
         <v>0</v>
       </c>
-      <c r="QZ27">
-        <v>102.75240658218445</v>
-      </c>
     </row>
-    <row r="28" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>382</v>
       </c>
@@ -41436,11 +41355,8 @@
       <c r="QY28">
         <v>1</v>
       </c>
-      <c r="QZ28">
-        <v>103.00189209842549</v>
-      </c>
     </row>
-    <row r="29" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>383</v>
       </c>
@@ -42843,11 +42759,8 @@
       <c r="QY29">
         <v>0</v>
       </c>
-      <c r="QZ29">
-        <v>104.35624227285329</v>
-      </c>
     </row>
-    <row r="30" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>384</v>
       </c>
@@ -44250,11 +44163,8 @@
       <c r="QY30">
         <v>0</v>
       </c>
-      <c r="QZ30">
-        <v>105.10469892849876</v>
-      </c>
     </row>
-    <row r="31" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>385</v>
       </c>
@@ -45657,11 +45567,8 @@
       <c r="QY31">
         <v>0</v>
       </c>
-      <c r="QZ31">
-        <v>105.28290292976943</v>
-      </c>
     </row>
-    <row r="32" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>386</v>
       </c>
@@ -47084,11 +46991,8 @@
       <c r="QY32">
         <v>1</v>
       </c>
-      <c r="QZ32">
-        <v>105.3185436872546</v>
-      </c>
     </row>
-    <row r="33" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>387</v>
       </c>
@@ -48511,11 +48415,8 @@
       <c r="QY33">
         <v>0</v>
       </c>
-      <c r="QZ33">
-        <v>105.56802920349563</v>
-      </c>
     </row>
-    <row r="34" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -49938,11 +49839,8 @@
       <c r="QY34">
         <v>0</v>
       </c>
-      <c r="QZ34">
-        <v>105.99571872100734</v>
-      </c>
     </row>
-    <row r="35" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>389</v>
       </c>
@@ -51365,11 +51263,8 @@
       <c r="QY35">
         <v>0</v>
       </c>
-      <c r="QZ35">
-        <v>105.81751482665905</v>
-      </c>
     </row>
-    <row r="36" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>390</v>
       </c>
@@ -52792,11 +52687,8 @@
       <c r="QY36">
         <v>1</v>
       </c>
-      <c r="QZ36">
-        <v>105.99571872100734</v>
-      </c>
     </row>
-    <row r="37" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>391</v>
       </c>
@@ -54219,11 +54111,8 @@
       <c r="QY37">
         <v>0</v>
       </c>
-      <c r="QZ37">
-        <v>106.20956347976319</v>
-      </c>
     </row>
-    <row r="38" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>392</v>
       </c>
@@ -55646,11 +55535,8 @@
       <c r="QY38">
         <v>0</v>
       </c>
-      <c r="QZ38">
-        <v>106.63725299727486</v>
-      </c>
     </row>
-    <row r="39" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>393</v>
       </c>
@@ -57073,11 +56959,8 @@
       <c r="QY39">
         <v>0</v>
       </c>
-      <c r="QZ39">
-        <v>106.42340823851902</v>
-      </c>
     </row>
-    <row r="40" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>394</v>
       </c>
@@ -58500,11 +58383,8 @@
       <c r="QY40">
         <v>1</v>
       </c>
-      <c r="QZ40">
-        <v>106.49468986041177</v>
-      </c>
     </row>
-    <row r="41" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -59927,11 +59807,8 @@
       <c r="QY41">
         <v>0</v>
       </c>
-      <c r="QZ41">
-        <v>106.49468986041177</v>
-      </c>
     </row>
-    <row r="42" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>396</v>
       </c>
@@ -61354,11 +61231,8 @@
       <c r="QY42">
         <v>0</v>
       </c>
-      <c r="QZ42">
-        <v>107.27878695277528</v>
-      </c>
     </row>
-    <row r="43" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>397</v>
       </c>
@@ -62781,11 +62655,8 @@
       <c r="QY43">
         <v>0</v>
       </c>
-      <c r="QZ43">
-        <v>107.06494219401941</v>
-      </c>
     </row>
-    <row r="44" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>398</v>
       </c>
@@ -64208,11 +64079,8 @@
       <c r="QY44">
         <v>1</v>
       </c>
-      <c r="QZ44">
-        <v>106.85109775603071</v>
-      </c>
     </row>
-    <row r="45" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>399</v>
       </c>
@@ -65635,11 +65503,8 @@
       <c r="QY45">
         <v>0</v>
       </c>
-      <c r="QZ45">
-        <v>106.81545699854553</v>
-      </c>
     </row>
-    <row r="46" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>400</v>
       </c>
@@ -67062,11 +66927,8 @@
       <c r="QY46">
         <v>0</v>
       </c>
-      <c r="QZ46">
-        <v>107.42135083809502</v>
-      </c>
     </row>
-    <row r="47" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>401</v>
       </c>
@@ -68489,11 +68351,8 @@
       <c r="QY47">
         <v>0</v>
       </c>
-      <c r="QZ47">
-        <v>107.24314651605722</v>
-      </c>
     </row>
-    <row r="48" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -69916,11 +69775,8 @@
       <c r="QY48">
         <v>1</v>
       </c>
-      <c r="QZ48">
-        <v>107.27878695277528</v>
-      </c>
     </row>
-    <row r="49" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>403</v>
       </c>
@@ -71343,11 +71199,8 @@
       <c r="QY49">
         <v>0</v>
       </c>
-      <c r="QZ49">
-        <v>107.84904035560675</v>
-      </c>
     </row>
-    <row r="50" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>404</v>
       </c>
@@ -72770,11 +72623,8 @@
       <c r="QY50">
         <v>0</v>
       </c>
-      <c r="QZ50">
-        <v>108.31237030983647</v>
-      </c>
     </row>
-    <row r="51" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -74197,11 +74047,8 @@
       <c r="QY51">
         <v>0</v>
       </c>
-      <c r="QZ51">
-        <v>108.88262264344412</v>
-      </c>
     </row>
-    <row r="52" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>406</v>
       </c>
@@ -75624,11 +75471,8 @@
       <c r="QY52">
         <v>1</v>
       </c>
-      <c r="QZ52">
-        <v>108.63313744797023</v>
-      </c>
     </row>
-    <row r="53" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>407</v>
       </c>
@@ -77051,11 +76895,8 @@
       <c r="QY53">
         <v>0</v>
       </c>
-      <c r="QZ53">
-        <v>108.49057463187427</v>
-      </c>
     </row>
-    <row r="54" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>408</v>
       </c>
@@ -78479,11 +78320,8 @@
       <c r="QY54">
         <v>0</v>
       </c>
-      <c r="QZ54">
-        <v>109.3815941036157</v>
-      </c>
     </row>
-    <row r="55" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -79907,11 +79745,8 @@
       <c r="QY55">
         <v>0</v>
       </c>
-      <c r="QZ55">
-        <v>109.84492405784543</v>
-      </c>
     </row>
-    <row r="56" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>410</v>
       </c>
@@ -81335,11 +81170,8 @@
       <c r="QY56">
         <v>1</v>
       </c>
-      <c r="QZ56">
-        <v>109.48851648299362</v>
-      </c>
     </row>
-    <row r="57" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>411</v>
       </c>
@@ -82763,11 +82595,8 @@
       <c r="QY57">
         <v>0</v>
       </c>
-      <c r="QZ57">
-        <v>109.77364318440935</v>
-      </c>
     </row>
-    <row r="58" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>412</v>
       </c>
@@ -84191,11 +84020,8 @@
       <c r="QY58">
         <v>0</v>
       </c>
-      <c r="QZ58">
-        <v>110.20133270192103</v>
-      </c>
     </row>
-    <row r="59" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>413</v>
       </c>
@@ -85619,11 +85445,8 @@
       <c r="QY59">
         <v>0</v>
       </c>
-      <c r="QZ59">
-        <v>110.30825508129897</v>
-      </c>
     </row>
-    <row r="60" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>414</v>
       </c>
@@ -87047,11 +86870,8 @@
       <c r="QY60">
         <v>1</v>
       </c>
-      <c r="QZ60">
-        <v>110.23697313863909</v>
-      </c>
     </row>
-    <row r="61" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>415</v>
       </c>
@@ -88475,11 +88295,8 @@
       <c r="QY61">
         <v>0</v>
       </c>
-      <c r="QZ61">
-        <v>110.45081789739493</v>
-      </c>
     </row>
-    <row r="62" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF62" s="1"/>
       <c r="LG62" s="1"/>
       <c r="LH62" s="1"/>
@@ -88525,7 +88342,7 @@
       <c r="QF62" s="5"/>
       <c r="QK62" s="6"/>
     </row>
-    <row r="63" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF63" s="1"/>
       <c r="LG63" s="1"/>
       <c r="LH63" s="1"/>
@@ -88571,7 +88388,7 @@
       <c r="QF63" s="5"/>
       <c r="QK63" s="6"/>
     </row>
-    <row r="64" spans="1:468" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:467" ht="15.75" x14ac:dyDescent="0.25">
       <c r="LF64" s="1"/>
       <c r="LG64" s="1"/>
       <c r="LH64" s="1"/>

</xml_diff>